<commit_message>
v1.1 campo para moneda y ajustes de int()
</commit_message>
<xml_diff>
--- a/bdpl/SP.xlsx
+++ b/bdpl/SP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.herrera\programmingProjects\ofertaElectroInterfaz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.herrera\programmingProjects\ofertaElectroInterfaz\bdpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A084F41C-52CA-43FD-8A39-64A7361595B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D322796-49A0-4114-9D90-E81AE2BD535E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1890" windowWidth="29040" windowHeight="15720" xr2:uid="{D648EDC0-5B86-4BF2-94F1-4B01206086EC}"/>
+    <workbookView xWindow="20370" yWindow="-1890" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D648EDC0-5B86-4BF2-94F1-4B01206086EC}"/>
   </bookViews>
   <sheets>
     <sheet name="SOLICITUD" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="135">
   <si>
     <t>ESTAMPILLAS</t>
   </si>
@@ -443,6 +443,18 @@
   </si>
   <si>
     <t xml:space="preserve">TIQUETES </t>
+  </si>
+  <si>
+    <t>LA OFERTA SE REQUIERE EN</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>INSUMOS TÉCNICOS ADICIONALES</t>
+  </si>
+  <si>
+    <t>Observaciones:</t>
   </si>
 </sst>
 </file>
@@ -457,10 +469,10 @@
     <numFmt numFmtId="167" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0.00\ [$€]_-;\-* #,##0.00\ [$€]_-;_-* &quot;-&quot;??\ [$€]_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="_-[$$-240A]\ * #,##0_-;\-[$$-240A]\ * #,##0_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="[$$-240A]\ #,##0.00"/>
-    <numFmt numFmtId="173" formatCode="[$$-240A]\ #,##0"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="[$$-240A]\ #,##0.00"/>
+    <numFmt numFmtId="172" formatCode="[$$-240A]\ #,##0"/>
+    <numFmt numFmtId="173" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -655,7 +667,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -875,6 +887,113 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -887,7 +1006,7 @@
     <xf numFmtId="43" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1002,9 +1121,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="21" fillId="3" borderId="18" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1014,13 +1130,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="22" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="22" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="22" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="22" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="23" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="23" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1047,12 +1163,27 @@
     <xf numFmtId="2" fontId="15" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="171" fontId="17" fillId="6" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="172" fontId="17" fillId="6" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="17" fillId="6" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="173" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1085,6 +1216,48 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1520,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BFF3BA-D898-4517-B0F1-00F08A29B046}">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1563,26 +1736,26 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="61" t="s">
+      <c r="G3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="69"/>
     </row>
     <row r="4" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="66"/>
       <c r="E4" s="10">
-        <f>GASTOS!F21</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="66"/>
+        <f>GASTOS!F22</f>
+        <v>4485960</v>
+      </c>
+      <c r="G4" s="70"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="72"/>
       <c r="M4" s="2"/>
       <c r="N4" s="3"/>
     </row>
@@ -1592,10 +1765,10 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="10"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="66"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
     </row>
     <row r="6" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="7" t="s">
@@ -1603,10 +1776,10 @@
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="11"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="66"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="72"/>
     </row>
     <row r="7" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="7" t="s">
@@ -1616,10 +1789,10 @@
       <c r="E7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="64"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="66"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="72"/>
     </row>
     <row r="8" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="7" t="s">
@@ -1627,10 +1800,10 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="12"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="66"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="72"/>
     </row>
     <row r="9" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="7" t="s">
@@ -1638,10 +1811,10 @@
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="12"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="66"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="72"/>
     </row>
     <row r="10" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="7" t="s">
@@ -1649,10 +1822,10 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="12"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="66"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="72"/>
     </row>
     <row r="11" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="7" t="s">
@@ -1660,10 +1833,10 @@
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="12"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="66"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="72"/>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1674,10 +1847,10 @@
       <c r="E12" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="64"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="66"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="72"/>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.2">
@@ -1686,10 +1859,10 @@
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="12"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="66"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="72"/>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.2">
@@ -1697,13 +1870,13 @@
         <v>13</v>
       </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="64"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="66"/>
+      <c r="E14" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="70"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="72"/>
       <c r="L14" s="2"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -1714,20 +1887,21 @@
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="12"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="69"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="75"/>
       <c r="L15" s="2"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="3:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="14" t="s">
+    <row r="16" spans="3:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="63"/>
       <c r="G16" s="17" t="s">
         <v>16</v>
       </c>
@@ -1738,7 +1912,15 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="76" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17" s="77"/>
+      <c r="E17" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="63"/>
       <c r="M17" s="18"/>
       <c r="O17" s="2"/>
       <c r="P17" s="3"/>
@@ -1749,6 +1931,7 @@
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
+      <c r="F18" s="64"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
@@ -1811,7 +1994,7 @@
       <c r="H20" s="40"/>
       <c r="I20" s="41"/>
       <c r="J20" s="24"/>
-      <c r="K20" s="42"/>
+      <c r="K20" s="58"/>
       <c r="L20" s="25"/>
       <c r="M20" s="26"/>
     </row>
@@ -1826,7 +2009,7 @@
       <c r="H21" s="40"/>
       <c r="I21" s="41"/>
       <c r="J21" s="24"/>
-      <c r="K21" s="42"/>
+      <c r="K21" s="58"/>
       <c r="L21" s="25"/>
       <c r="M21" s="26"/>
     </row>
@@ -1841,7 +2024,7 @@
       <c r="H22" s="40"/>
       <c r="I22" s="41"/>
       <c r="J22" s="24"/>
-      <c r="K22" s="42"/>
+      <c r="K22" s="58"/>
       <c r="L22" s="25"/>
       <c r="M22" s="26"/>
     </row>
@@ -1856,7 +2039,7 @@
       <c r="H23" s="40"/>
       <c r="I23" s="41"/>
       <c r="J23" s="24"/>
-      <c r="K23" s="42"/>
+      <c r="K23" s="58"/>
       <c r="L23" s="25"/>
       <c r="M23" s="26"/>
     </row>
@@ -1871,7 +2054,7 @@
       <c r="H24" s="40"/>
       <c r="I24" s="41"/>
       <c r="J24" s="24"/>
-      <c r="K24" s="42"/>
+      <c r="K24" s="58"/>
       <c r="L24" s="25"/>
       <c r="M24" s="26"/>
     </row>
@@ -1886,7 +2069,7 @@
       <c r="H25" s="40"/>
       <c r="I25" s="41"/>
       <c r="J25" s="24"/>
-      <c r="K25" s="42"/>
+      <c r="K25" s="58"/>
       <c r="L25" s="25"/>
       <c r="M25" s="26"/>
     </row>
@@ -1901,7 +2084,7 @@
       <c r="H26" s="40"/>
       <c r="I26" s="41"/>
       <c r="J26" s="24"/>
-      <c r="K26" s="42"/>
+      <c r="K26" s="58"/>
       <c r="L26" s="25"/>
       <c r="M26" s="26"/>
     </row>
@@ -1916,7 +2099,7 @@
       <c r="H27" s="40"/>
       <c r="I27" s="41"/>
       <c r="J27" s="24"/>
-      <c r="K27" s="42"/>
+      <c r="K27" s="58"/>
       <c r="L27" s="25"/>
       <c r="M27" s="26"/>
     </row>
@@ -1931,7 +2114,7 @@
       <c r="H28" s="40"/>
       <c r="I28" s="41"/>
       <c r="J28" s="24"/>
-      <c r="K28" s="42"/>
+      <c r="K28" s="58"/>
       <c r="L28" s="25"/>
       <c r="M28" s="26"/>
     </row>
@@ -1946,7 +2129,7 @@
       <c r="H29" s="40"/>
       <c r="I29" s="41"/>
       <c r="J29" s="24"/>
-      <c r="K29" s="42"/>
+      <c r="K29" s="58"/>
       <c r="L29" s="25"/>
       <c r="M29" s="26"/>
     </row>
@@ -1961,7 +2144,7 @@
       <c r="H30" s="40"/>
       <c r="I30" s="41"/>
       <c r="J30" s="24"/>
-      <c r="K30" s="42"/>
+      <c r="K30" s="58"/>
       <c r="L30" s="25"/>
       <c r="M30" s="26"/>
     </row>
@@ -1976,7 +2159,7 @@
       <c r="H31" s="40"/>
       <c r="I31" s="41"/>
       <c r="J31" s="24"/>
-      <c r="K31" s="42"/>
+      <c r="K31" s="58"/>
       <c r="L31" s="25"/>
       <c r="M31" s="26"/>
     </row>
@@ -1991,7 +2174,7 @@
       <c r="H32" s="40"/>
       <c r="I32" s="41"/>
       <c r="J32" s="24"/>
-      <c r="K32" s="42"/>
+      <c r="K32" s="58"/>
       <c r="L32" s="25"/>
       <c r="M32" s="26"/>
     </row>
@@ -2006,7 +2189,7 @@
       <c r="H33" s="40"/>
       <c r="I33" s="41"/>
       <c r="J33" s="24"/>
-      <c r="K33" s="42"/>
+      <c r="K33" s="58"/>
       <c r="L33" s="25"/>
       <c r="M33" s="26"/>
     </row>
@@ -2021,7 +2204,7 @@
       <c r="H34" s="40"/>
       <c r="I34" s="41"/>
       <c r="J34" s="24"/>
-      <c r="K34" s="42"/>
+      <c r="K34" s="58"/>
       <c r="L34" s="25"/>
       <c r="M34" s="26"/>
     </row>
@@ -2036,7 +2219,7 @@
       <c r="H35" s="40"/>
       <c r="I35" s="41"/>
       <c r="J35" s="24"/>
-      <c r="K35" s="42"/>
+      <c r="K35" s="58"/>
       <c r="L35" s="25"/>
       <c r="M35" s="26"/>
     </row>
@@ -2051,7 +2234,7 @@
       <c r="H36" s="40"/>
       <c r="I36" s="41"/>
       <c r="J36" s="24"/>
-      <c r="K36" s="42"/>
+      <c r="K36" s="58"/>
       <c r="L36" s="25"/>
       <c r="M36" s="26"/>
     </row>
@@ -2066,7 +2249,7 @@
       <c r="H37" s="40"/>
       <c r="I37" s="41"/>
       <c r="J37" s="24"/>
-      <c r="K37" s="42"/>
+      <c r="K37" s="58"/>
       <c r="L37" s="25"/>
       <c r="M37" s="26"/>
     </row>
@@ -2081,7 +2264,7 @@
       <c r="H38" s="40"/>
       <c r="I38" s="41"/>
       <c r="J38" s="24"/>
-      <c r="K38" s="42"/>
+      <c r="K38" s="58"/>
       <c r="L38" s="25"/>
       <c r="M38" s="26"/>
     </row>
@@ -2096,7 +2279,7 @@
       <c r="H39" s="40"/>
       <c r="I39" s="41"/>
       <c r="J39" s="24"/>
-      <c r="K39" s="42"/>
+      <c r="K39" s="58"/>
       <c r="L39" s="25"/>
       <c r="M39" s="26"/>
     </row>
@@ -2111,7 +2294,7 @@
       <c r="H40" s="40"/>
       <c r="I40" s="41"/>
       <c r="J40" s="24"/>
-      <c r="K40" s="42"/>
+      <c r="K40" s="58"/>
       <c r="L40" s="25"/>
       <c r="M40" s="26"/>
     </row>
@@ -2126,7 +2309,7 @@
       <c r="H41" s="40"/>
       <c r="I41" s="41"/>
       <c r="J41" s="24"/>
-      <c r="K41" s="42"/>
+      <c r="K41" s="58"/>
       <c r="L41" s="25"/>
       <c r="M41" s="26"/>
     </row>
@@ -2141,7 +2324,7 @@
       <c r="H42" s="40"/>
       <c r="I42" s="41"/>
       <c r="J42" s="24"/>
-      <c r="K42" s="42"/>
+      <c r="K42" s="58"/>
       <c r="L42" s="25"/>
       <c r="M42" s="26"/>
     </row>
@@ -2156,7 +2339,7 @@
       <c r="H43" s="40"/>
       <c r="I43" s="41"/>
       <c r="J43" s="24"/>
-      <c r="K43" s="42"/>
+      <c r="K43" s="58"/>
       <c r="L43" s="25"/>
       <c r="M43" s="26"/>
     </row>
@@ -2171,7 +2354,7 @@
       <c r="H44" s="40"/>
       <c r="I44" s="41"/>
       <c r="J44" s="24"/>
-      <c r="K44" s="42"/>
+      <c r="K44" s="58"/>
       <c r="L44" s="25"/>
       <c r="M44" s="26"/>
     </row>
@@ -2186,7 +2369,7 @@
       <c r="H45" s="40"/>
       <c r="I45" s="41"/>
       <c r="J45" s="24"/>
-      <c r="K45" s="42"/>
+      <c r="K45" s="58"/>
       <c r="L45" s="25"/>
       <c r="M45" s="26"/>
     </row>
@@ -2201,7 +2384,7 @@
       <c r="H46" s="40"/>
       <c r="I46" s="41"/>
       <c r="J46" s="24"/>
-      <c r="K46" s="42"/>
+      <c r="K46" s="58"/>
       <c r="L46" s="25"/>
       <c r="M46" s="26"/>
     </row>
@@ -2216,7 +2399,7 @@
       <c r="H47" s="40"/>
       <c r="I47" s="41"/>
       <c r="J47" s="24"/>
-      <c r="K47" s="42"/>
+      <c r="K47" s="58"/>
       <c r="L47" s="25"/>
       <c r="M47" s="26"/>
     </row>
@@ -2231,7 +2414,7 @@
       <c r="H48" s="40"/>
       <c r="I48" s="41"/>
       <c r="J48" s="24"/>
-      <c r="K48" s="42"/>
+      <c r="K48" s="58"/>
       <c r="L48" s="25"/>
       <c r="M48" s="26"/>
     </row>
@@ -2246,7 +2429,7 @@
       <c r="H49" s="40"/>
       <c r="I49" s="41"/>
       <c r="J49" s="24"/>
-      <c r="K49" s="42"/>
+      <c r="K49" s="58"/>
       <c r="L49" s="25"/>
       <c r="M49" s="26"/>
     </row>
@@ -2261,7 +2444,7 @@
       <c r="H50" s="40"/>
       <c r="I50" s="41"/>
       <c r="J50" s="24"/>
-      <c r="K50" s="42"/>
+      <c r="K50" s="58"/>
       <c r="L50" s="25"/>
       <c r="M50" s="26"/>
     </row>
@@ -2276,7 +2459,7 @@
       <c r="H51" s="40"/>
       <c r="I51" s="41"/>
       <c r="J51" s="24"/>
-      <c r="K51" s="42"/>
+      <c r="K51" s="58"/>
       <c r="L51" s="25"/>
       <c r="M51" s="26"/>
     </row>
@@ -2291,7 +2474,7 @@
       <c r="H52" s="40"/>
       <c r="I52" s="41"/>
       <c r="J52" s="24"/>
-      <c r="K52" s="42"/>
+      <c r="K52" s="58"/>
       <c r="L52" s="25"/>
       <c r="M52" s="26"/>
     </row>
@@ -2306,7 +2489,7 @@
       <c r="H53" s="40"/>
       <c r="I53" s="41"/>
       <c r="J53" s="24"/>
-      <c r="K53" s="42"/>
+      <c r="K53" s="58"/>
       <c r="L53" s="25"/>
       <c r="M53" s="26"/>
     </row>
@@ -2321,7 +2504,7 @@
       <c r="H54" s="40"/>
       <c r="I54" s="41"/>
       <c r="J54" s="24"/>
-      <c r="K54" s="42"/>
+      <c r="K54" s="58"/>
       <c r="L54" s="25"/>
       <c r="M54" s="26"/>
     </row>
@@ -2336,7 +2519,7 @@
       <c r="H55" s="40"/>
       <c r="I55" s="41"/>
       <c r="J55" s="24"/>
-      <c r="K55" s="42"/>
+      <c r="K55" s="58"/>
       <c r="L55" s="25"/>
       <c r="M55" s="26"/>
     </row>
@@ -2351,7 +2534,7 @@
       <c r="H56" s="40"/>
       <c r="I56" s="41"/>
       <c r="J56" s="24"/>
-      <c r="K56" s="42"/>
+      <c r="K56" s="58"/>
       <c r="L56" s="25"/>
       <c r="M56" s="26"/>
     </row>
@@ -2366,7 +2549,7 @@
       <c r="H57" s="40"/>
       <c r="I57" s="41"/>
       <c r="J57" s="24"/>
-      <c r="K57" s="42"/>
+      <c r="K57" s="58"/>
       <c r="L57" s="25"/>
       <c r="M57" s="26"/>
     </row>
@@ -2381,7 +2564,7 @@
       <c r="H58" s="40"/>
       <c r="I58" s="41"/>
       <c r="J58" s="24"/>
-      <c r="K58" s="42"/>
+      <c r="K58" s="58"/>
       <c r="L58" s="25"/>
       <c r="M58" s="26"/>
     </row>
@@ -2396,7 +2579,7 @@
       <c r="H59" s="40"/>
       <c r="I59" s="41"/>
       <c r="J59" s="24"/>
-      <c r="K59" s="42"/>
+      <c r="K59" s="58"/>
       <c r="L59" s="25"/>
       <c r="M59" s="26"/>
     </row>
@@ -2411,7 +2594,7 @@
       <c r="H60" s="40"/>
       <c r="I60" s="41"/>
       <c r="J60" s="24"/>
-      <c r="K60" s="42"/>
+      <c r="K60" s="58"/>
       <c r="L60" s="25"/>
       <c r="M60" s="26"/>
     </row>
@@ -2426,7 +2609,7 @@
       <c r="H61" s="40"/>
       <c r="I61" s="41"/>
       <c r="J61" s="24"/>
-      <c r="K61" s="42"/>
+      <c r="K61" s="58"/>
       <c r="L61" s="25"/>
       <c r="M61" s="26"/>
     </row>
@@ -2441,7 +2624,7 @@
       <c r="H62" s="40"/>
       <c r="I62" s="41"/>
       <c r="J62" s="24"/>
-      <c r="K62" s="42"/>
+      <c r="K62" s="58"/>
       <c r="L62" s="25"/>
       <c r="M62" s="26"/>
     </row>
@@ -2456,7 +2639,7 @@
       <c r="H63" s="40"/>
       <c r="I63" s="41"/>
       <c r="J63" s="24"/>
-      <c r="K63" s="42"/>
+      <c r="K63" s="58"/>
       <c r="L63" s="25"/>
       <c r="M63" s="26"/>
     </row>
@@ -2471,7 +2654,7 @@
       <c r="H64" s="40"/>
       <c r="I64" s="41"/>
       <c r="J64" s="24"/>
-      <c r="K64" s="42"/>
+      <c r="K64" s="58"/>
       <c r="L64" s="25"/>
       <c r="M64" s="26"/>
     </row>
@@ -2486,7 +2669,7 @@
       <c r="H65" s="40"/>
       <c r="I65" s="41"/>
       <c r="J65" s="24"/>
-      <c r="K65" s="42"/>
+      <c r="K65" s="58"/>
       <c r="L65" s="25"/>
       <c r="M65" s="26"/>
     </row>
@@ -2501,7 +2684,7 @@
       <c r="H66" s="40"/>
       <c r="I66" s="41"/>
       <c r="J66" s="24"/>
-      <c r="K66" s="42"/>
+      <c r="K66" s="58"/>
       <c r="L66" s="25"/>
       <c r="M66" s="26"/>
     </row>
@@ -2516,7 +2699,7 @@
       <c r="H67" s="40"/>
       <c r="I67" s="41"/>
       <c r="J67" s="24"/>
-      <c r="K67" s="42"/>
+      <c r="K67" s="58"/>
       <c r="L67" s="25"/>
       <c r="M67" s="26"/>
     </row>
@@ -2531,7 +2714,7 @@
       <c r="H68" s="40"/>
       <c r="I68" s="41"/>
       <c r="J68" s="24"/>
-      <c r="K68" s="42"/>
+      <c r="K68" s="58"/>
       <c r="L68" s="25"/>
       <c r="M68" s="26"/>
     </row>
@@ -2546,7 +2729,7 @@
       <c r="H69" s="40"/>
       <c r="I69" s="41"/>
       <c r="J69" s="24"/>
-      <c r="K69" s="42"/>
+      <c r="K69" s="58"/>
       <c r="L69" s="25"/>
       <c r="M69" s="26"/>
     </row>
@@ -2561,7 +2744,7 @@
       <c r="H70" s="40"/>
       <c r="I70" s="41"/>
       <c r="J70" s="24"/>
-      <c r="K70" s="42"/>
+      <c r="K70" s="58"/>
       <c r="L70" s="25"/>
       <c r="M70" s="26"/>
     </row>
@@ -2576,7 +2759,7 @@
       <c r="H71" s="40"/>
       <c r="I71" s="41"/>
       <c r="J71" s="24"/>
-      <c r="K71" s="42"/>
+      <c r="K71" s="58"/>
       <c r="L71" s="25"/>
       <c r="M71" s="26"/>
     </row>
@@ -2591,7 +2774,7 @@
       <c r="H72" s="40"/>
       <c r="I72" s="41"/>
       <c r="J72" s="24"/>
-      <c r="K72" s="42"/>
+      <c r="K72" s="58"/>
       <c r="L72" s="25"/>
       <c r="M72" s="26"/>
     </row>
@@ -2606,7 +2789,7 @@
       <c r="H73" s="40"/>
       <c r="I73" s="41"/>
       <c r="J73" s="24"/>
-      <c r="K73" s="42"/>
+      <c r="K73" s="58"/>
       <c r="L73" s="25"/>
       <c r="M73" s="26"/>
     </row>
@@ -2621,7 +2804,7 @@
       <c r="H74" s="40"/>
       <c r="I74" s="41"/>
       <c r="J74" s="24"/>
-      <c r="K74" s="42"/>
+      <c r="K74" s="58"/>
       <c r="L74" s="25"/>
       <c r="M74" s="26"/>
     </row>
@@ -2636,7 +2819,7 @@
       <c r="H75" s="40"/>
       <c r="I75" s="41"/>
       <c r="J75" s="24"/>
-      <c r="K75" s="42"/>
+      <c r="K75" s="58"/>
       <c r="L75" s="25"/>
       <c r="M75" s="26"/>
     </row>
@@ -2651,7 +2834,7 @@
       <c r="H76" s="40"/>
       <c r="I76" s="41"/>
       <c r="J76" s="24"/>
-      <c r="K76" s="42"/>
+      <c r="K76" s="58"/>
       <c r="L76" s="25"/>
       <c r="M76" s="26"/>
     </row>
@@ -2666,7 +2849,7 @@
       <c r="H77" s="40"/>
       <c r="I77" s="41"/>
       <c r="J77" s="24"/>
-      <c r="K77" s="42"/>
+      <c r="K77" s="58"/>
       <c r="L77" s="25"/>
       <c r="M77" s="26"/>
     </row>
@@ -2681,7 +2864,7 @@
       <c r="H78" s="40"/>
       <c r="I78" s="41"/>
       <c r="J78" s="24"/>
-      <c r="K78" s="42"/>
+      <c r="K78" s="58"/>
       <c r="L78" s="25"/>
       <c r="M78" s="26"/>
     </row>
@@ -2696,7 +2879,7 @@
       <c r="H79" s="40"/>
       <c r="I79" s="41"/>
       <c r="J79" s="24"/>
-      <c r="K79" s="42"/>
+      <c r="K79" s="58"/>
       <c r="L79" s="25"/>
       <c r="M79" s="26"/>
     </row>
@@ -2711,7 +2894,7 @@
       <c r="H80" s="40"/>
       <c r="I80" s="41"/>
       <c r="J80" s="24"/>
-      <c r="K80" s="42"/>
+      <c r="K80" s="58"/>
       <c r="L80" s="25"/>
       <c r="M80" s="26"/>
     </row>
@@ -2726,7 +2909,7 @@
       <c r="H81" s="40"/>
       <c r="I81" s="41"/>
       <c r="J81" s="24"/>
-      <c r="K81" s="42"/>
+      <c r="K81" s="58"/>
       <c r="L81" s="25"/>
       <c r="M81" s="26"/>
     </row>
@@ -2741,7 +2924,7 @@
       <c r="H82" s="40"/>
       <c r="I82" s="41"/>
       <c r="J82" s="24"/>
-      <c r="K82" s="42"/>
+      <c r="K82" s="58"/>
       <c r="L82" s="25"/>
       <c r="M82" s="26"/>
     </row>
@@ -2756,7 +2939,7 @@
       <c r="H83" s="40"/>
       <c r="I83" s="41"/>
       <c r="J83" s="24"/>
-      <c r="K83" s="42"/>
+      <c r="K83" s="58"/>
       <c r="L83" s="25"/>
       <c r="M83" s="26"/>
     </row>
@@ -2771,7 +2954,7 @@
       <c r="H84" s="40"/>
       <c r="I84" s="41"/>
       <c r="J84" s="24"/>
-      <c r="K84" s="42"/>
+      <c r="K84" s="58"/>
       <c r="L84" s="25"/>
       <c r="M84" s="26"/>
     </row>
@@ -2786,7 +2969,7 @@
       <c r="H85" s="40"/>
       <c r="I85" s="41"/>
       <c r="J85" s="24"/>
-      <c r="K85" s="42"/>
+      <c r="K85" s="58"/>
       <c r="L85" s="25"/>
       <c r="M85" s="26"/>
     </row>
@@ -2801,7 +2984,7 @@
       <c r="H86" s="40"/>
       <c r="I86" s="41"/>
       <c r="J86" s="24"/>
-      <c r="K86" s="42"/>
+      <c r="K86" s="58"/>
       <c r="L86" s="25"/>
       <c r="M86" s="26"/>
     </row>
@@ -2816,7 +2999,7 @@
       <c r="H87" s="40"/>
       <c r="I87" s="41"/>
       <c r="J87" s="24"/>
-      <c r="K87" s="42"/>
+      <c r="K87" s="58"/>
       <c r="L87" s="25"/>
       <c r="M87" s="26"/>
     </row>
@@ -2831,7 +3014,7 @@
       <c r="H88" s="40"/>
       <c r="I88" s="41"/>
       <c r="J88" s="24"/>
-      <c r="K88" s="42"/>
+      <c r="K88" s="58"/>
       <c r="L88" s="25"/>
       <c r="M88" s="26"/>
     </row>
@@ -2846,7 +3029,7 @@
       <c r="H89" s="40"/>
       <c r="I89" s="41"/>
       <c r="J89" s="24"/>
-      <c r="K89" s="42"/>
+      <c r="K89" s="58"/>
       <c r="L89" s="25"/>
       <c r="M89" s="26"/>
     </row>
@@ -2861,7 +3044,7 @@
       <c r="H90" s="40"/>
       <c r="I90" s="41"/>
       <c r="J90" s="24"/>
-      <c r="K90" s="42"/>
+      <c r="K90" s="58"/>
       <c r="L90" s="25"/>
       <c r="M90" s="26"/>
     </row>
@@ -2876,7 +3059,7 @@
       <c r="H91" s="40"/>
       <c r="I91" s="41"/>
       <c r="J91" s="24"/>
-      <c r="K91" s="42"/>
+      <c r="K91" s="58"/>
       <c r="L91" s="25"/>
       <c r="M91" s="26"/>
     </row>
@@ -2891,7 +3074,7 @@
       <c r="H92" s="40"/>
       <c r="I92" s="41"/>
       <c r="J92" s="24"/>
-      <c r="K92" s="42"/>
+      <c r="K92" s="58"/>
       <c r="L92" s="25"/>
       <c r="M92" s="26"/>
     </row>
@@ -2906,7 +3089,7 @@
       <c r="H93" s="40"/>
       <c r="I93" s="41"/>
       <c r="J93" s="24"/>
-      <c r="K93" s="42"/>
+      <c r="K93" s="58"/>
       <c r="L93" s="25"/>
       <c r="M93" s="26"/>
     </row>
@@ -2921,7 +3104,7 @@
       <c r="H94" s="40"/>
       <c r="I94" s="41"/>
       <c r="J94" s="24"/>
-      <c r="K94" s="42"/>
+      <c r="K94" s="58"/>
       <c r="L94" s="25"/>
       <c r="M94" s="26"/>
     </row>
@@ -2936,7 +3119,7 @@
       <c r="H95" s="40"/>
       <c r="I95" s="41"/>
       <c r="J95" s="24"/>
-      <c r="K95" s="42"/>
+      <c r="K95" s="58"/>
       <c r="L95" s="25"/>
       <c r="M95" s="26"/>
     </row>
@@ -2951,7 +3134,7 @@
       <c r="H96" s="40"/>
       <c r="I96" s="41"/>
       <c r="J96" s="24"/>
-      <c r="K96" s="42"/>
+      <c r="K96" s="58"/>
       <c r="L96" s="25"/>
       <c r="M96" s="26"/>
     </row>
@@ -2966,7 +3149,7 @@
       <c r="H97" s="40"/>
       <c r="I97" s="41"/>
       <c r="J97" s="24"/>
-      <c r="K97" s="42"/>
+      <c r="K97" s="58"/>
       <c r="L97" s="25"/>
       <c r="M97" s="26"/>
     </row>
@@ -2981,7 +3164,7 @@
       <c r="H98" s="40"/>
       <c r="I98" s="41"/>
       <c r="J98" s="24"/>
-      <c r="K98" s="42"/>
+      <c r="K98" s="58"/>
       <c r="L98" s="25"/>
       <c r="M98" s="26"/>
     </row>
@@ -2996,7 +3179,7 @@
       <c r="H99" s="40"/>
       <c r="I99" s="41"/>
       <c r="J99" s="24"/>
-      <c r="K99" s="42"/>
+      <c r="K99" s="58"/>
       <c r="L99" s="25"/>
       <c r="M99" s="26"/>
     </row>
@@ -3011,7 +3194,7 @@
       <c r="H100" s="40"/>
       <c r="I100" s="41"/>
       <c r="J100" s="24"/>
-      <c r="K100" s="42"/>
+      <c r="K100" s="58"/>
       <c r="L100" s="25"/>
       <c r="M100" s="26"/>
     </row>
@@ -3026,7 +3209,7 @@
       <c r="H101" s="40"/>
       <c r="I101" s="41"/>
       <c r="J101" s="24"/>
-      <c r="K101" s="42"/>
+      <c r="K101" s="58"/>
       <c r="L101" s="25"/>
       <c r="M101" s="26"/>
     </row>
@@ -3041,7 +3224,7 @@
       <c r="H102" s="40"/>
       <c r="I102" s="41"/>
       <c r="J102" s="24"/>
-      <c r="K102" s="42"/>
+      <c r="K102" s="58"/>
       <c r="L102" s="25"/>
       <c r="M102" s="26"/>
     </row>
@@ -3056,7 +3239,7 @@
       <c r="H103" s="40"/>
       <c r="I103" s="41"/>
       <c r="J103" s="24"/>
-      <c r="K103" s="42"/>
+      <c r="K103" s="58"/>
       <c r="L103" s="25"/>
       <c r="M103" s="26"/>
     </row>
@@ -3071,7 +3254,7 @@
       <c r="H104" s="40"/>
       <c r="I104" s="41"/>
       <c r="J104" s="24"/>
-      <c r="K104" s="42"/>
+      <c r="K104" s="58"/>
       <c r="L104" s="25"/>
       <c r="M104" s="26"/>
     </row>
@@ -3086,17 +3269,18 @@
       <c r="H105" s="40"/>
       <c r="I105" s="41"/>
       <c r="J105" s="24"/>
-      <c r="K105" s="42"/>
+      <c r="K105" s="58"/>
       <c r="L105" s="25"/>
       <c r="M105" s="26"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="G3:J15"/>
+    <mergeCell ref="C17:D17"/>
   </mergeCells>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G20:G105" xr:uid="{1E861047-1092-4F41-9DB4-E7B836CEF09C}">
       <formula1>"Nacional, Internacional, Inventario"</formula1>
     </dataValidation>
@@ -3121,6 +3305,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12" xr:uid="{8F2B761D-1150-4F18-ACCB-51F17E22E067}">
       <formula1>"DAVID HERRERA,JOAN PORRAS,NICOLAS HERRERA, ANDRES BOHORQUEZ,WILMER CRUZ,JORGE RODRIGUEZ,CRISTIAN MUÑOZ"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17" xr:uid="{59EF5DC7-822A-43C1-97EA-29B50D4E6053}">
+      <formula1>"COP,USD,EUR"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3141,10 +3328,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A82BDF-4B1A-4248-B7D7-0A123242CAD7}">
-  <dimension ref="C6:F21"/>
+  <dimension ref="C6:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3153,46 +3340,47 @@
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="53">
-        <v>0</v>
+      <c r="D6" s="52">
+        <v>5</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="52" t="str">
+      <c r="F6" s="51" t="str">
         <f>SOLICITUD!E14</f>
-        <v>ACACÍAS</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>BUCARAMANGA</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="53">
-        <v>0</v>
+      <c r="D7" s="52">
+        <v>2</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="29"/>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
       <c r="F8" s="29"/>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
       <c r="F9" s="29"/>
     </row>
-    <row r="10" spans="3:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C10" s="30" t="s">
         <v>55</v>
       </c>
@@ -3205,117 +3393,143 @@
       <c r="F10" s="32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="H10" s="78" t="s">
+        <v>134</v>
+      </c>
+      <c r="I10" s="81"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="83"/>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="54">
+      <c r="D11" s="53">
         <v>1</v>
       </c>
       <c r="E11" s="34">
         <f>VLOOKUP(F6,TARIFAS!A:I,2,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="57">
+        <v>830180</v>
+      </c>
+      <c r="F11" s="56">
         <f>D11*E11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>830180</v>
+      </c>
+      <c r="H11" s="79"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="86"/>
+    </row>
+    <row r="12" spans="3:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="54">
+      <c r="D12" s="53">
         <v>1</v>
       </c>
       <c r="E12" s="34">
         <f>VLOOKUP(F6,TARIFAS!A:I,3,FALSE)</f>
         <v>70000</v>
       </c>
-      <c r="F12" s="57">
+      <c r="F12" s="56">
         <f t="shared" ref="F12:F13" si="0">D12*E12</f>
         <v>70000</v>
       </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="H12" s="79"/>
+      <c r="I12" s="84"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="86"/>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C13" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="54">
+      <c r="D13" s="53">
         <v>1</v>
       </c>
       <c r="E13" s="34">
         <f>VLOOKUP(F6,TARIFAS!A:I,4,FALSE)</f>
-        <v>30000</v>
-      </c>
-      <c r="F13" s="57">
+        <v>90000</v>
+      </c>
+      <c r="F13" s="56">
         <f t="shared" si="0"/>
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+        <v>90000</v>
+      </c>
+      <c r="H13" s="79"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="86"/>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C14" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="54">
+      <c r="D14" s="53">
         <f>D6</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E14" s="35">
         <f>VLOOKUP(F6,TARIFAS!A:I,5,FALSE)</f>
         <v>60000</v>
       </c>
-      <c r="F14" s="57">
+      <c r="F14" s="56">
         <f>D14*E14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+        <v>300000</v>
+      </c>
+      <c r="H14" s="79"/>
+      <c r="I14" s="84"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="86"/>
+    </row>
+    <row r="15" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="53">
         <v>1</v>
       </c>
       <c r="E15" s="34">
         <f>VLOOKUP(F6,TARIFAS!A:I,6,FALSE)</f>
-        <v>92000</v>
-      </c>
-      <c r="F15" s="57">
+        <v>0</v>
+      </c>
+      <c r="F15" s="56">
         <f>D15*E15</f>
-        <v>92000</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H15" s="80"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="89"/>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="56">
+      <c r="D16" s="55">
         <f>IF(D7&lt;1,0,4*D6/D7)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E16" s="36">
         <f>VLOOKUP(F6,TARIFAS!A:I,7,FALSE)</f>
-        <v>15000</v>
-      </c>
-      <c r="F16" s="58">
+        <v>20000</v>
+      </c>
+      <c r="F16" s="57">
         <f>D16*E16</f>
-        <v>0</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="54">
+      <c r="D17" s="53">
         <v>1</v>
       </c>
       <c r="E17" s="36">
         <f>VLOOKUP(F6,TARIFAS!A:I,8,FALSE)</f>
         <v>15000</v>
       </c>
-      <c r="F17" s="57">
+      <c r="F17" s="56">
         <f>D17*E17</f>
         <v>15000</v>
       </c>
@@ -3324,45 +3538,67 @@
       <c r="C18" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="D18" s="54">
+      <c r="D18" s="53">
         <f>D6-1</f>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="E18" s="36">
         <f>VLOOKUP(F6,TARIFAS!A:I,9,FALSE)</f>
-        <v>96000</v>
-      </c>
-      <c r="F18" s="57">
+        <v>184450</v>
+      </c>
+      <c r="F18" s="56">
         <f>IF(D18&lt;0,0,E18*D18)</f>
-        <v>0</v>
+        <v>737800</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-    </row>
-    <row r="20" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C19" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="53">
+        <v>0</v>
+      </c>
+      <c r="E19" s="36">
+        <v>0</v>
+      </c>
+      <c r="F19" s="56">
+        <f>D19*E19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="28"/>
       <c r="D20" s="28"/>
-      <c r="E20" s="31" t="s">
+    </row>
+    <row r="21" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="37">
+      <c r="F21" s="37">
         <f>SUM(F11:F18)</f>
-        <v>207000</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E21" s="31" t="s">
+        <v>2242980</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E22" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="37">
-        <f>F20*D7</f>
-        <v>0</v>
+      <c r="F22" s="37">
+        <f>(F21*D7)+F19</f>
+        <v>4485960</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H10:H15"/>
+    <mergeCell ref="I10:K15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F18" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -3371,1643 +3607,1643 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="51" customWidth="1"/>
-    <col min="2" max="2" width="18" style="51" customWidth="1"/>
-    <col min="3" max="3" width="29" style="51" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="51" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" style="51" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="51" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="51" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="51" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" style="51" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="50" customWidth="1"/>
+    <col min="2" max="2" width="18" style="50" customWidth="1"/>
+    <col min="3" max="3" width="29" style="50" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="50" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="50" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="50" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="50" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="50" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="42" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="46">
-        <v>0</v>
-      </c>
-      <c r="C2" s="46">
+      <c r="B2" s="45">
+        <v>0</v>
+      </c>
+      <c r="C2" s="45">
         <f t="shared" ref="C2:C34" si="0">35000*2</f>
         <v>70000</v>
       </c>
-      <c r="D2" s="47">
+      <c r="D2" s="46">
         <v>30000</v>
       </c>
-      <c r="E2" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F2" s="46">
+      <c r="E2" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F2" s="45">
         <v>92000</v>
       </c>
-      <c r="G2" s="46">
+      <c r="G2" s="45">
         <v>15000</v>
       </c>
-      <c r="H2" s="46">
+      <c r="H2" s="45">
         <v>15000</v>
       </c>
-      <c r="I2" s="46">
+      <c r="I2" s="45">
         <v>96000</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="45">
         <v>700000</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D3" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E3" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F3" s="46">
-        <v>0</v>
-      </c>
-      <c r="G3" s="46">
+      <c r="D3" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E3" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F3" s="45">
+        <v>0</v>
+      </c>
+      <c r="G3" s="45">
         <v>10000</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="45">
         <v>15000</v>
       </c>
-      <c r="I3" s="46">
+      <c r="I3" s="45">
         <v>105000</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="46">
-        <v>0</v>
-      </c>
-      <c r="C4" s="46">
+      <c r="B4" s="45">
+        <v>0</v>
+      </c>
+      <c r="C4" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="46">
         <v>20000</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="45">
         <v>35000</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="45">
         <v>40000</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="45">
         <v>10000</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <v>15000</v>
       </c>
-      <c r="I4" s="46">
+      <c r="I4" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>1218100</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D5" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E5" s="46">
-        <v>70000</v>
-      </c>
-      <c r="F5" s="46">
-        <v>0</v>
-      </c>
-      <c r="G5" s="46">
+      <c r="D5" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E5" s="45">
+        <v>70000</v>
+      </c>
+      <c r="F5" s="45">
+        <v>0</v>
+      </c>
+      <c r="G5" s="45">
         <v>15000</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <v>51000</v>
       </c>
-      <c r="I5" s="46">
+      <c r="I5" s="45">
         <v>190000</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="46">
-        <v>0</v>
-      </c>
-      <c r="C6" s="46">
+      <c r="B6" s="45">
+        <v>0</v>
+      </c>
+      <c r="C6" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="46">
         <v>20000</v>
       </c>
-      <c r="E6" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F6" s="46">
+      <c r="E6" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F6" s="45">
         <v>40000</v>
       </c>
-      <c r="G6" s="46">
+      <c r="G6" s="45">
         <v>10000</v>
       </c>
-      <c r="H6" s="46">
+      <c r="H6" s="45">
         <v>15000</v>
       </c>
-      <c r="I6" s="46">
+      <c r="I6" s="45">
         <v>50000</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>772900</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D7" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E7" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F7" s="46">
-        <v>0</v>
-      </c>
-      <c r="G7" s="46">
+      <c r="D7" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E7" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F7" s="45">
+        <v>0</v>
+      </c>
+      <c r="G7" s="45">
         <v>20000</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H7" s="45">
         <v>15000</v>
       </c>
-      <c r="I7" s="46">
+      <c r="I7" s="45">
         <v>169000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.3">
-      <c r="A8" s="45" t="s">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="46">
-        <v>0</v>
-      </c>
-      <c r="C8" s="46">
+      <c r="B8" s="45">
+        <v>0</v>
+      </c>
+      <c r="C8" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D8" s="47">
-        <v>0</v>
-      </c>
-      <c r="E8" s="46">
-        <v>0</v>
-      </c>
-      <c r="F8" s="46">
-        <v>0</v>
-      </c>
-      <c r="G8" s="46">
-        <v>0</v>
-      </c>
-      <c r="H8" s="46">
-        <v>0</v>
-      </c>
-      <c r="I8" s="46">
+      <c r="D8" s="46">
+        <v>0</v>
+      </c>
+      <c r="E8" s="45">
+        <v>0</v>
+      </c>
+      <c r="F8" s="45">
+        <v>0</v>
+      </c>
+      <c r="G8" s="45">
+        <v>0</v>
+      </c>
+      <c r="H8" s="45">
+        <v>0</v>
+      </c>
+      <c r="I8" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>735080</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D9" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E9" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F9" s="46">
-        <v>0</v>
-      </c>
-      <c r="G9" s="46">
+      <c r="D9" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E9" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F9" s="45">
+        <v>0</v>
+      </c>
+      <c r="G9" s="45">
         <v>20000</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <v>15000</v>
       </c>
-      <c r="I9" s="46">
+      <c r="I9" s="45">
         <v>226100</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="46">
-        <v>0</v>
-      </c>
-      <c r="C10" s="46">
+      <c r="B10" s="45">
+        <v>0</v>
+      </c>
+      <c r="C10" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="46">
         <f>25000*2</f>
         <v>50000</v>
       </c>
-      <c r="E10" s="46">
-        <v>0</v>
-      </c>
-      <c r="F10" s="46">
-        <v>0</v>
-      </c>
-      <c r="G10" s="46">
-        <v>0</v>
-      </c>
-      <c r="H10" s="46">
-        <v>0</v>
-      </c>
-      <c r="I10" s="46">
+      <c r="E10" s="45">
+        <v>0</v>
+      </c>
+      <c r="F10" s="45">
+        <v>0</v>
+      </c>
+      <c r="G10" s="45">
+        <v>0</v>
+      </c>
+      <c r="H10" s="45">
+        <v>0</v>
+      </c>
+      <c r="I10" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>830180</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="46">
         <f>45000*2</f>
         <v>90000</v>
       </c>
-      <c r="E11" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F11" s="46">
-        <v>0</v>
-      </c>
-      <c r="G11" s="46">
+      <c r="E11" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F11" s="45">
+        <v>0</v>
+      </c>
+      <c r="G11" s="45">
         <v>20000</v>
       </c>
-      <c r="H11" s="46">
+      <c r="H11" s="45">
         <v>15000</v>
       </c>
-      <c r="I11" s="46">
+      <c r="I11" s="45">
         <v>184450</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="46">
-        <v>0</v>
-      </c>
-      <c r="C12" s="46">
+      <c r="B12" s="45">
+        <v>0</v>
+      </c>
+      <c r="C12" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="46">
         <v>30000</v>
       </c>
-      <c r="E12" s="46">
+      <c r="E12" s="45">
         <v>35000</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="45">
         <v>25000</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="45">
         <v>10000</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>15000</v>
       </c>
-      <c r="I12" s="46">
+      <c r="I12" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="45">
         <v>584680</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="46">
         <f>75000*2</f>
         <v>150000</v>
       </c>
-      <c r="E13" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F13" s="46">
-        <v>0</v>
-      </c>
-      <c r="G13" s="46">
+      <c r="E13" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F13" s="45">
+        <v>0</v>
+      </c>
+      <c r="G13" s="45">
         <v>20000</v>
       </c>
-      <c r="H13" s="46">
+      <c r="H13" s="45">
         <v>15000</v>
       </c>
-      <c r="I13" s="46">
+      <c r="I13" s="45">
         <v>178500</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="45">
         <v>1037930</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="46">
         <f>25000*2</f>
         <v>50000</v>
       </c>
-      <c r="E14" s="46">
-        <v>70000</v>
-      </c>
-      <c r="F14" s="46">
-        <v>0</v>
-      </c>
-      <c r="G14" s="46">
+      <c r="E14" s="45">
+        <v>70000</v>
+      </c>
+      <c r="F14" s="45">
+        <v>0</v>
+      </c>
+      <c r="G14" s="45">
         <v>20000</v>
       </c>
-      <c r="H14" s="46">
+      <c r="H14" s="45">
         <v>15000</v>
       </c>
-      <c r="I14" s="46">
+      <c r="I14" s="45">
         <v>226100</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="46">
-        <v>0</v>
-      </c>
-      <c r="C15" s="46">
+      <c r="B15" s="45">
+        <v>0</v>
+      </c>
+      <c r="C15" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="46">
         <v>30000</v>
       </c>
-      <c r="E15" s="46">
+      <c r="E15" s="45">
         <v>35000</v>
       </c>
-      <c r="F15" s="46">
+      <c r="F15" s="45">
         <v>25000</v>
       </c>
-      <c r="G15" s="46">
+      <c r="G15" s="45">
         <v>10000</v>
       </c>
-      <c r="H15" s="46">
+      <c r="H15" s="45">
         <v>15000</v>
       </c>
-      <c r="I15" s="46">
+      <c r="I15" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="46">
-        <v>0</v>
-      </c>
-      <c r="C16" s="46">
+      <c r="B16" s="45">
+        <v>0</v>
+      </c>
+      <c r="C16" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D16" s="47">
-        <v>0</v>
-      </c>
-      <c r="E16" s="46">
-        <v>0</v>
-      </c>
-      <c r="F16" s="46">
-        <v>0</v>
-      </c>
-      <c r="G16" s="46">
-        <v>0</v>
-      </c>
-      <c r="H16" s="46">
-        <v>0</v>
-      </c>
-      <c r="I16" s="46">
+      <c r="D16" s="46">
+        <v>0</v>
+      </c>
+      <c r="E16" s="45">
+        <v>0</v>
+      </c>
+      <c r="F16" s="45">
+        <v>0</v>
+      </c>
+      <c r="G16" s="45">
+        <v>0</v>
+      </c>
+      <c r="H16" s="45">
+        <v>0</v>
+      </c>
+      <c r="I16" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="46">
-        <v>0</v>
-      </c>
-      <c r="C17" s="46">
+      <c r="B17" s="45">
+        <v>0</v>
+      </c>
+      <c r="C17" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D17" s="47">
-        <v>0</v>
-      </c>
-      <c r="E17" s="46">
-        <v>0</v>
-      </c>
-      <c r="F17" s="46">
-        <v>0</v>
-      </c>
-      <c r="G17" s="46">
-        <v>0</v>
-      </c>
-      <c r="H17" s="46">
-        <v>0</v>
-      </c>
-      <c r="I17" s="46">
+      <c r="D17" s="46">
+        <v>0</v>
+      </c>
+      <c r="E17" s="45">
+        <v>0</v>
+      </c>
+      <c r="F17" s="45">
+        <v>0</v>
+      </c>
+      <c r="G17" s="45">
+        <v>0</v>
+      </c>
+      <c r="H17" s="45">
+        <v>0</v>
+      </c>
+      <c r="I17" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="B18" s="46">
+      <c r="B18" s="45">
         <v>801500</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D18" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E18" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F18" s="46">
-        <v>0</v>
-      </c>
-      <c r="G18" s="46">
+      <c r="D18" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E18" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F18" s="45">
+        <v>0</v>
+      </c>
+      <c r="G18" s="45">
         <v>20000</v>
       </c>
-      <c r="H18" s="46">
+      <c r="H18" s="45">
         <v>15000</v>
       </c>
-      <c r="I18" s="46">
+      <c r="I18" s="45">
         <v>190400</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="48">
+      <c r="B19" s="47">
         <v>808680</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C19" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D19" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E19" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F19" s="46">
-        <v>0</v>
-      </c>
-      <c r="G19" s="46">
+      <c r="D19" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E19" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F19" s="45">
+        <v>0</v>
+      </c>
+      <c r="G19" s="45">
         <v>10000</v>
       </c>
-      <c r="H19" s="46">
+      <c r="H19" s="45">
         <v>15000</v>
       </c>
-      <c r="I19" s="46">
+      <c r="I19" s="45">
         <v>184450</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="46">
-        <v>0</v>
-      </c>
-      <c r="C20" s="46">
+      <c r="B20" s="45">
+        <v>0</v>
+      </c>
+      <c r="C20" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D20" s="46">
         <v>30000</v>
       </c>
-      <c r="E20" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F20" s="46">
+      <c r="E20" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F20" s="45">
         <v>80000</v>
       </c>
-      <c r="G20" s="46">
+      <c r="G20" s="45">
         <v>10000</v>
       </c>
-      <c r="H20" s="46">
+      <c r="H20" s="45">
         <v>15000</v>
       </c>
-      <c r="I20" s="46">
+      <c r="I20" s="45">
         <v>115000</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="46">
-        <v>0</v>
-      </c>
-      <c r="C21" s="46">
+      <c r="B21" s="45">
+        <v>0</v>
+      </c>
+      <c r="C21" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D21" s="47">
+      <c r="D21" s="46">
         <v>20000</v>
       </c>
-      <c r="E21" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F21" s="46">
+      <c r="E21" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F21" s="45">
         <v>80000</v>
       </c>
-      <c r="G21" s="46">
+      <c r="G21" s="45">
         <v>10000</v>
       </c>
-      <c r="H21" s="46">
+      <c r="H21" s="45">
         <v>15000</v>
       </c>
-      <c r="I21" s="46">
+      <c r="I21" s="45">
         <v>110000</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="46">
-        <v>0</v>
-      </c>
-      <c r="C22" s="46">
+      <c r="B22" s="45">
+        <v>0</v>
+      </c>
+      <c r="C22" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="46">
         <v>30000</v>
       </c>
-      <c r="E22" s="46">
+      <c r="E22" s="45">
         <v>35000</v>
       </c>
-      <c r="F22" s="46">
+      <c r="F22" s="45">
         <v>25000</v>
       </c>
-      <c r="G22" s="46">
+      <c r="G22" s="45">
         <v>10000</v>
       </c>
-      <c r="H22" s="46">
+      <c r="H22" s="45">
         <v>15000</v>
       </c>
-      <c r="I22" s="46">
+      <c r="I22" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="46">
+      <c r="B23" s="45">
         <v>1111800</v>
       </c>
-      <c r="C23" s="46">
+      <c r="C23" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D23" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E23" s="46">
-        <v>70000</v>
-      </c>
-      <c r="F23" s="46">
-        <v>0</v>
-      </c>
-      <c r="G23" s="46">
+      <c r="D23" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E23" s="45">
+        <v>70000</v>
+      </c>
+      <c r="F23" s="45">
+        <v>0</v>
+      </c>
+      <c r="G23" s="45">
         <v>20000</v>
       </c>
-      <c r="H23" s="46">
+      <c r="H23" s="45">
         <v>15000</v>
       </c>
-      <c r="I23" s="46">
+      <c r="I23" s="45">
         <v>140000</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="46">
-        <v>0</v>
-      </c>
-      <c r="C24" s="46">
+      <c r="B24" s="45">
+        <v>0</v>
+      </c>
+      <c r="C24" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D24" s="47">
+      <c r="D24" s="46">
         <v>30000</v>
       </c>
-      <c r="E24" s="46">
+      <c r="E24" s="45">
         <v>35000</v>
       </c>
-      <c r="F24" s="46">
+      <c r="F24" s="45">
         <v>40000</v>
       </c>
-      <c r="G24" s="46">
+      <c r="G24" s="45">
         <v>10000</v>
       </c>
-      <c r="H24" s="46">
+      <c r="H24" s="45">
         <v>15000</v>
       </c>
-      <c r="I24" s="46">
+      <c r="I24" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="46">
-        <v>0</v>
-      </c>
-      <c r="C25" s="46">
+      <c r="B25" s="45">
+        <v>0</v>
+      </c>
+      <c r="C25" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D25" s="47">
+      <c r="D25" s="46">
         <v>20000</v>
       </c>
-      <c r="E25" s="46">
+      <c r="E25" s="45">
         <v>35000</v>
       </c>
-      <c r="F25" s="46">
-        <v>0</v>
-      </c>
-      <c r="G25" s="46">
+      <c r="F25" s="45">
+        <v>0</v>
+      </c>
+      <c r="G25" s="45">
         <v>10000</v>
       </c>
-      <c r="H25" s="46">
+      <c r="H25" s="45">
         <v>15000</v>
       </c>
-      <c r="I25" s="46">
+      <c r="I25" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="46">
-        <v>0</v>
-      </c>
-      <c r="C26" s="46">
+      <c r="B26" s="45">
+        <v>0</v>
+      </c>
+      <c r="C26" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D26" s="47">
+      <c r="D26" s="46">
         <v>30000</v>
       </c>
-      <c r="E26" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F26" s="46">
+      <c r="E26" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F26" s="45">
         <v>80000</v>
       </c>
-      <c r="G26" s="46">
+      <c r="G26" s="45">
         <v>15000</v>
       </c>
-      <c r="H26" s="46">
+      <c r="H26" s="45">
         <v>15000</v>
       </c>
-      <c r="I26" s="46">
+      <c r="I26" s="45">
         <v>100000</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="45" t="s">
+      <c r="A27" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="46">
-        <v>0</v>
-      </c>
-      <c r="C27" s="46">
+      <c r="B27" s="45">
+        <v>0</v>
+      </c>
+      <c r="C27" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="46">
         <v>40000</v>
       </c>
-      <c r="E27" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F27" s="46">
+      <c r="E27" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F27" s="45">
         <v>100000</v>
       </c>
-      <c r="G27" s="46">
+      <c r="G27" s="45">
         <v>15000</v>
       </c>
-      <c r="H27" s="46">
+      <c r="H27" s="45">
         <v>15000</v>
       </c>
-      <c r="I27" s="46">
+      <c r="I27" s="45">
         <v>205000</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="46">
-        <v>0</v>
-      </c>
-      <c r="C28" s="46">
+      <c r="B28" s="45">
+        <v>0</v>
+      </c>
+      <c r="C28" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D28" s="47">
-        <v>0</v>
-      </c>
-      <c r="E28" s="46">
-        <v>0</v>
-      </c>
-      <c r="F28" s="46">
-        <v>0</v>
-      </c>
-      <c r="G28" s="46">
-        <v>0</v>
-      </c>
-      <c r="H28" s="46">
-        <v>0</v>
-      </c>
-      <c r="I28" s="46">
+      <c r="D28" s="46">
+        <v>0</v>
+      </c>
+      <c r="E28" s="45">
+        <v>0</v>
+      </c>
+      <c r="F28" s="45">
+        <v>0</v>
+      </c>
+      <c r="G28" s="45">
+        <v>0</v>
+      </c>
+      <c r="H28" s="45">
+        <v>0</v>
+      </c>
+      <c r="I28" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="46">
+      <c r="B29" s="45">
         <v>718850</v>
       </c>
-      <c r="C29" s="46">
+      <c r="C29" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D29" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E29" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F29" s="46">
-        <v>0</v>
-      </c>
-      <c r="G29" s="46">
+      <c r="D29" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E29" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F29" s="45">
+        <v>0</v>
+      </c>
+      <c r="G29" s="45">
         <v>20000</v>
       </c>
-      <c r="H29" s="46">
+      <c r="H29" s="45">
         <v>15000</v>
       </c>
-      <c r="I29" s="46">
+      <c r="I29" s="45">
         <v>166600</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="46">
+      <c r="B30" s="45">
         <v>712980</v>
       </c>
-      <c r="C30" s="46">
+      <c r="C30" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D30" s="47">
+      <c r="D30" s="46">
         <f>100000*2</f>
         <v>200000</v>
       </c>
-      <c r="E30" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F30" s="46">
-        <v>0</v>
-      </c>
-      <c r="G30" s="46">
+      <c r="E30" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F30" s="45">
+        <v>0</v>
+      </c>
+      <c r="G30" s="45">
         <v>20000</v>
       </c>
-      <c r="H30" s="46">
+      <c r="H30" s="45">
         <v>15000</v>
       </c>
-      <c r="I30" s="46">
+      <c r="I30" s="45">
         <v>226100</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="46">
+      <c r="B31" s="45">
         <v>774260</v>
       </c>
-      <c r="C31" s="46">
+      <c r="C31" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D31" s="47">
+      <c r="D31" s="46">
         <f>30000*2</f>
         <v>60000</v>
       </c>
-      <c r="E31" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F31" s="46">
-        <v>0</v>
-      </c>
-      <c r="G31" s="46">
+      <c r="E31" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F31" s="45">
+        <v>0</v>
+      </c>
+      <c r="G31" s="45">
         <v>10000</v>
       </c>
-      <c r="H31" s="46">
+      <c r="H31" s="45">
         <v>15000</v>
       </c>
-      <c r="I31" s="46">
+      <c r="I31" s="45">
         <v>118000</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="46">
+      <c r="B32" s="45">
         <v>836550</v>
       </c>
-      <c r="C32" s="46">
+      <c r="C32" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D32" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E32" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F32" s="46">
-        <v>0</v>
-      </c>
-      <c r="G32" s="46">
+      <c r="D32" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E32" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F32" s="45">
+        <v>0</v>
+      </c>
+      <c r="G32" s="45">
         <v>20000</v>
       </c>
-      <c r="H32" s="46">
+      <c r="H32" s="45">
         <v>15000</v>
       </c>
-      <c r="I32" s="46">
+      <c r="I32" s="45">
         <v>160000</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="46">
-        <v>0</v>
-      </c>
-      <c r="C33" s="46">
+      <c r="B33" s="45">
+        <v>0</v>
+      </c>
+      <c r="C33" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D33" s="47">
+      <c r="D33" s="46">
         <v>20000</v>
       </c>
-      <c r="E33" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F33" s="46">
+      <c r="E33" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F33" s="45">
         <v>80000</v>
       </c>
-      <c r="G33" s="46">
+      <c r="G33" s="45">
         <v>10000</v>
       </c>
-      <c r="H33" s="46">
+      <c r="H33" s="45">
         <v>15000</v>
       </c>
-      <c r="I33" s="46">
+      <c r="I33" s="45">
         <v>113000</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="45" t="s">
+      <c r="A34" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="46">
+      <c r="B34" s="45">
         <v>657450</v>
       </c>
-      <c r="C34" s="46">
+      <c r="C34" s="45">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="D34" s="47">
+      <c r="D34" s="46">
         <v>80000</v>
       </c>
-      <c r="E34" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F34" s="46">
-        <v>0</v>
-      </c>
-      <c r="G34" s="46">
+      <c r="E34" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F34" s="45">
+        <v>0</v>
+      </c>
+      <c r="G34" s="45">
         <v>20000</v>
       </c>
-      <c r="H34" s="46">
+      <c r="H34" s="45">
         <v>15000</v>
       </c>
-      <c r="I34" s="46">
+      <c r="I34" s="45">
         <v>165000</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="46">
+      <c r="B35" s="45">
         <v>801500</v>
       </c>
-      <c r="C35" s="46">
-        <v>60000</v>
-      </c>
-      <c r="D35" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E35" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F35" s="46">
+      <c r="C35" s="45">
+        <v>60000</v>
+      </c>
+      <c r="D35" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E35" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F35" s="45">
         <v>35000</v>
       </c>
-      <c r="G35" s="46">
+      <c r="G35" s="45">
         <v>10000</v>
       </c>
-      <c r="H35" s="46">
-        <v>0</v>
-      </c>
-      <c r="I35" s="46">
+      <c r="H35" s="45">
+        <v>0</v>
+      </c>
+      <c r="I35" s="45">
         <v>130000</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="B36" s="46">
+      <c r="B36" s="45">
         <v>1201220</v>
       </c>
-      <c r="C36" s="46">
+      <c r="C36" s="45">
         <f t="shared" ref="C36:C54" si="1">35000*2</f>
         <v>70000</v>
       </c>
-      <c r="D36" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E36" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F36" s="46">
-        <v>0</v>
-      </c>
-      <c r="G36" s="46">
+      <c r="D36" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E36" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F36" s="45">
+        <v>0</v>
+      </c>
+      <c r="G36" s="45">
         <v>20000</v>
       </c>
-      <c r="H36" s="46">
+      <c r="H36" s="45">
         <v>15000</v>
       </c>
-      <c r="I36" s="46">
+      <c r="I36" s="45">
         <v>130900</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="45" t="s">
+      <c r="A37" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="B37" s="46">
+      <c r="B37" s="45">
         <v>718850</v>
       </c>
-      <c r="C37" s="46">
+      <c r="C37" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D37" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E37" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F37" s="46">
-        <v>0</v>
-      </c>
-      <c r="G37" s="46">
+      <c r="D37" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E37" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F37" s="45">
+        <v>0</v>
+      </c>
+      <c r="G37" s="45">
         <v>20000</v>
       </c>
-      <c r="H37" s="46">
+      <c r="H37" s="45">
         <v>15000</v>
       </c>
-      <c r="I37" s="46">
+      <c r="I37" s="45">
         <v>184450</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="46">
-        <v>0</v>
-      </c>
-      <c r="C38" s="46">
+      <c r="B38" s="45">
+        <v>0</v>
+      </c>
+      <c r="C38" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D38" s="47">
+      <c r="D38" s="46">
         <v>30000</v>
       </c>
-      <c r="E38" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F38" s="46">
-        <v>0</v>
-      </c>
-      <c r="G38" s="46">
+      <c r="E38" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F38" s="45">
+        <v>0</v>
+      </c>
+      <c r="G38" s="45">
         <v>10000</v>
       </c>
-      <c r="H38" s="46">
+      <c r="H38" s="45">
         <v>15000</v>
       </c>
-      <c r="I38" s="46">
+      <c r="I38" s="45">
         <v>120000</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="B39" s="46">
+      <c r="B39" s="45">
         <v>829610</v>
       </c>
-      <c r="C39" s="46">
+      <c r="C39" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D39" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E39" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F39" s="46">
-        <v>0</v>
-      </c>
-      <c r="G39" s="46">
+      <c r="D39" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E39" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F39" s="45">
+        <v>0</v>
+      </c>
+      <c r="G39" s="45">
         <v>20000</v>
       </c>
-      <c r="H39" s="46">
+      <c r="H39" s="45">
         <v>15000</v>
       </c>
-      <c r="I39" s="46">
+      <c r="I39" s="45">
         <v>226100</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="45" t="s">
+      <c r="A40" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="B40" s="46">
-        <v>0</v>
-      </c>
-      <c r="C40" s="46">
+      <c r="B40" s="45">
+        <v>0</v>
+      </c>
+      <c r="C40" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D40" s="47">
+      <c r="D40" s="46">
         <v>30000</v>
       </c>
-      <c r="E40" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F40" s="46">
-        <v>0</v>
-      </c>
-      <c r="G40" s="46">
+      <c r="E40" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F40" s="45">
+        <v>0</v>
+      </c>
+      <c r="G40" s="45">
         <v>10000</v>
       </c>
-      <c r="H40" s="46">
-        <v>0</v>
-      </c>
-      <c r="I40" s="46">
+      <c r="H40" s="45">
+        <v>0</v>
+      </c>
+      <c r="I40" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="B41" s="46">
+      <c r="B41" s="45">
         <v>795950</v>
       </c>
-      <c r="C41" s="46">
+      <c r="C41" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D41" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E41" s="46">
-        <v>70000</v>
-      </c>
-      <c r="F41" s="46">
-        <v>0</v>
-      </c>
-      <c r="G41" s="46">
+      <c r="D41" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E41" s="45">
+        <v>70000</v>
+      </c>
+      <c r="F41" s="45">
+        <v>0</v>
+      </c>
+      <c r="G41" s="45">
         <v>15000</v>
       </c>
-      <c r="H41" s="46">
+      <c r="H41" s="45">
         <v>15000</v>
       </c>
-      <c r="I41" s="46">
+      <c r="I41" s="45">
         <v>166897</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="45" t="s">
+      <c r="A42" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="46">
-        <v>0</v>
-      </c>
-      <c r="C42" s="46">
+      <c r="B42" s="45">
+        <v>0</v>
+      </c>
+      <c r="C42" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D42" s="47">
+      <c r="D42" s="46">
         <v>20000</v>
       </c>
-      <c r="E42" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F42" s="46">
+      <c r="E42" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F42" s="45">
         <v>80000</v>
       </c>
-      <c r="G42" s="46">
+      <c r="G42" s="45">
         <v>10000</v>
       </c>
-      <c r="H42" s="46">
+      <c r="H42" s="45">
         <v>15000</v>
       </c>
-      <c r="I42" s="46">
+      <c r="I42" s="45">
         <v>100000</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="45" t="s">
+      <c r="A43" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="46">
+      <c r="B43" s="45">
         <v>923800</v>
       </c>
-      <c r="C43" s="46">
+      <c r="C43" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D43" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E43" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F43" s="46">
-        <v>0</v>
-      </c>
-      <c r="G43" s="46">
+      <c r="D43" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E43" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F43" s="45">
+        <v>0</v>
+      </c>
+      <c r="G43" s="45">
         <v>20000</v>
       </c>
-      <c r="H43" s="46">
+      <c r="H43" s="45">
         <v>15000</v>
       </c>
-      <c r="I43" s="46">
+      <c r="I43" s="45">
         <v>142480</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="B44" s="46">
+      <c r="B44" s="45">
         <v>820940</v>
       </c>
-      <c r="C44" s="46">
+      <c r="C44" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D44" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E44" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F44" s="46">
-        <v>70000</v>
-      </c>
-      <c r="G44" s="46">
+      <c r="D44" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E44" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F44" s="45">
+        <v>70000</v>
+      </c>
+      <c r="G44" s="45">
         <v>10000</v>
       </c>
-      <c r="H44" s="46">
+      <c r="H44" s="45">
         <v>15000</v>
       </c>
-      <c r="I44" s="46">
+      <c r="I44" s="45">
         <v>110000</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="B45" s="46">
-        <v>0</v>
-      </c>
-      <c r="C45" s="46">
+      <c r="B45" s="45">
+        <v>0</v>
+      </c>
+      <c r="C45" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D45" s="47">
-        <v>0</v>
-      </c>
-      <c r="E45" s="46">
-        <v>0</v>
-      </c>
-      <c r="F45" s="46">
-        <v>0</v>
-      </c>
-      <c r="G45" s="46">
-        <v>0</v>
-      </c>
-      <c r="H45" s="46">
-        <v>0</v>
-      </c>
-      <c r="I45" s="46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.3">
-      <c r="A46" s="45" t="s">
+      <c r="D45" s="46">
+        <v>0</v>
+      </c>
+      <c r="E45" s="45">
+        <v>0</v>
+      </c>
+      <c r="F45" s="45">
+        <v>0</v>
+      </c>
+      <c r="G45" s="45">
+        <v>0</v>
+      </c>
+      <c r="H45" s="45">
+        <v>0</v>
+      </c>
+      <c r="I45" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="46">
+      <c r="B46" s="45">
         <v>852200</v>
       </c>
-      <c r="C46" s="46">
+      <c r="C46" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D46" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E46" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F46" s="46">
+      <c r="D46" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E46" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F46" s="45">
         <v>100000</v>
       </c>
-      <c r="G46" s="46">
+      <c r="G46" s="45">
         <v>10000</v>
       </c>
-      <c r="H46" s="46">
+      <c r="H46" s="45">
         <v>15000</v>
       </c>
-      <c r="I46" s="46">
+      <c r="I46" s="45">
         <v>110000</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="B47" s="46">
+      <c r="B47" s="45">
         <v>969280</v>
       </c>
-      <c r="C47" s="46">
+      <c r="C47" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D47" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E47" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F47" s="46">
-        <v>0</v>
-      </c>
-      <c r="G47" s="46">
+      <c r="D47" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E47" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F47" s="45">
+        <v>0</v>
+      </c>
+      <c r="G47" s="45">
         <v>20000</v>
       </c>
-      <c r="H47" s="47">
+      <c r="H47" s="46">
         <v>15000</v>
       </c>
-      <c r="I47" s="46">
+      <c r="I47" s="45">
         <v>220000</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="45" t="s">
+      <c r="A48" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="B48" s="46">
-        <v>0</v>
-      </c>
-      <c r="C48" s="46">
+      <c r="B48" s="45">
+        <v>0</v>
+      </c>
+      <c r="C48" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D48" s="47">
+      <c r="D48" s="46">
         <v>30000</v>
       </c>
-      <c r="E48" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F48" s="46">
+      <c r="E48" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F48" s="45">
         <v>90000</v>
       </c>
-      <c r="G48" s="46">
+      <c r="G48" s="45">
         <v>10000</v>
       </c>
-      <c r="H48" s="46">
+      <c r="H48" s="45">
         <v>15000</v>
       </c>
-      <c r="I48" s="46">
+      <c r="I48" s="45">
         <v>85800</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="45" t="s">
+      <c r="A49" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="46">
-        <v>0</v>
-      </c>
-      <c r="C49" s="46">
+      <c r="B49" s="45">
+        <v>0</v>
+      </c>
+      <c r="C49" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D49" s="47">
+      <c r="D49" s="46">
         <v>40000</v>
       </c>
-      <c r="E49" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F49" s="46">
+      <c r="E49" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F49" s="45">
         <v>80000</v>
       </c>
-      <c r="G49" s="46">
+      <c r="G49" s="45">
         <v>20000</v>
       </c>
-      <c r="H49" s="46">
+      <c r="H49" s="45">
         <v>15000</v>
       </c>
-      <c r="I49" s="46">
+      <c r="I49" s="45">
         <v>119000</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="B50" s="46">
-        <v>0</v>
-      </c>
-      <c r="C50" s="46">
+      <c r="B50" s="45">
+        <v>0</v>
+      </c>
+      <c r="C50" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D50" s="47">
-        <v>0</v>
-      </c>
-      <c r="E50" s="46">
-        <v>0</v>
-      </c>
-      <c r="F50" s="46">
-        <v>0</v>
-      </c>
-      <c r="G50" s="46">
-        <v>0</v>
-      </c>
-      <c r="H50" s="46">
-        <v>0</v>
-      </c>
-      <c r="I50" s="46">
+      <c r="D50" s="46">
+        <v>0</v>
+      </c>
+      <c r="E50" s="45">
+        <v>0</v>
+      </c>
+      <c r="F50" s="45">
+        <v>0</v>
+      </c>
+      <c r="G50" s="45">
+        <v>0</v>
+      </c>
+      <c r="H50" s="45">
+        <v>0</v>
+      </c>
+      <c r="I50" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="B51" s="46">
+      <c r="B51" s="45">
         <v>804120</v>
       </c>
-      <c r="C51" s="46">
+      <c r="C51" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D51" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E51" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F51" s="46">
-        <v>0</v>
-      </c>
-      <c r="G51" s="46">
+      <c r="D51" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E51" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F51" s="45">
+        <v>0</v>
+      </c>
+      <c r="G51" s="45">
         <v>20000</v>
       </c>
-      <c r="H51" s="46">
+      <c r="H51" s="45">
         <v>15000</v>
       </c>
-      <c r="I51" s="46">
+      <c r="I51" s="45">
         <v>154700</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="45" t="s">
+      <c r="A52" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="B52" s="46">
-        <v>0</v>
-      </c>
-      <c r="C52" s="46">
+      <c r="B52" s="45">
+        <v>0</v>
+      </c>
+      <c r="C52" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D52" s="47">
+      <c r="D52" s="46">
         <v>20000</v>
       </c>
-      <c r="E52" s="46">
+      <c r="E52" s="45">
         <v>35000</v>
       </c>
-      <c r="F52" s="46">
+      <c r="F52" s="45">
         <v>40000</v>
       </c>
-      <c r="G52" s="46">
+      <c r="G52" s="45">
         <v>10000</v>
       </c>
-      <c r="H52" s="46">
+      <c r="H52" s="45">
         <v>15000</v>
       </c>
-      <c r="I52" s="46">
+      <c r="I52" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="45" t="s">
+      <c r="A53" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="B53" s="46">
+      <c r="B53" s="45">
         <v>574350</v>
       </c>
-      <c r="C53" s="46">
+      <c r="C53" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D53" s="47">
-        <v>60000</v>
-      </c>
-      <c r="E53" s="46">
-        <v>60000</v>
-      </c>
-      <c r="F53" s="46">
-        <v>0</v>
-      </c>
-      <c r="G53" s="46">
+      <c r="D53" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E53" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F53" s="45">
+        <v>0</v>
+      </c>
+      <c r="G53" s="45">
         <v>20000</v>
       </c>
-      <c r="H53" s="46">
+      <c r="H53" s="45">
         <v>15000</v>
       </c>
-      <c r="I53" s="46">
+      <c r="I53" s="45">
         <v>90000</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="50" t="s">
+      <c r="A54" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="B54" s="46">
-        <v>0</v>
-      </c>
-      <c r="C54" s="46">
+      <c r="B54" s="45">
+        <v>0</v>
+      </c>
+      <c r="C54" s="45">
         <f t="shared" si="1"/>
         <v>70000</v>
       </c>
-      <c r="D54" s="47">
+      <c r="D54" s="46">
         <v>30000</v>
       </c>
-      <c r="E54" s="46">
+      <c r="E54" s="45">
         <v>35000</v>
       </c>
-      <c r="F54" s="46">
+      <c r="F54" s="45">
         <v>25000</v>
       </c>
-      <c r="G54" s="46">
+      <c r="G54" s="45">
         <v>10000</v>
       </c>
-      <c r="H54" s="46">
+      <c r="H54" s="45">
         <v>15000</v>
       </c>
-      <c r="I54" s="46">
+      <c r="I54" s="45">
         <v>0</v>
       </c>
     </row>
@@ -5031,19 +5267,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
     </row>
     <row r="4" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="3:13" x14ac:dyDescent="0.25">
@@ -5067,10 +5303,10 @@
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="60"/>
+      <c r="D7" s="66"/>
       <c r="E7" s="10"/>
       <c r="F7" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
v1.2 se arreglaron campos de porcentajes y bugs con cantidades cuando no hay items
</commit_message>
<xml_diff>
--- a/bdpl/SP.xlsx
+++ b/bdpl/SP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.herrera\programmingProjects\ofertaElectroInterfaz\bdpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D322796-49A0-4114-9D90-E81AE2BD535E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1A14E8-BE70-43B1-93DE-9D41B650D611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1890" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D648EDC0-5B86-4BF2-94F1-4B01206086EC}"/>
+    <workbookView xWindow="20370" yWindow="-1890" windowWidth="29040" windowHeight="15720" xr2:uid="{D648EDC0-5B86-4BF2-94F1-4B01206086EC}"/>
   </bookViews>
   <sheets>
     <sheet name="SOLICITUD" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="137">
   <si>
     <t>ESTAMPILLAS</t>
   </si>
@@ -448,13 +448,19 @@
     <t>LA OFERTA SE REQUIERE EN</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
     <t>INSUMOS TÉCNICOS ADICIONALES</t>
   </si>
   <si>
     <t>Observaciones:</t>
+  </si>
+  <si>
+    <t>VILLAVICENCIO</t>
+  </si>
+  <si>
+    <t>PUERTO BERRIO</t>
+  </si>
+  <si>
+    <t>SINCELEJO</t>
   </si>
 </sst>
 </file>
@@ -474,7 +480,7 @@
     <numFmt numFmtId="172" formatCode="[$$-240A]\ #,##0"/>
     <numFmt numFmtId="173" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -628,6 +634,19 @@
       <sz val="10"/>
       <name val="Montserrat Light"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Montserrat Light"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -667,7 +686,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -994,6 +1013,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1006,7 +1038,7 @@
     <xf numFmtId="43" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1184,6 +1216,22 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="170" fontId="24" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="24" fillId="0" borderId="28" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="24" fillId="0" borderId="28" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1693,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BFF3BA-D898-4517-B0F1-00F08A29B046}">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1736,26 +1784,26 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="75"/>
     </row>
     <row r="4" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="10">
+      <c r="D4" s="72"/>
+      <c r="E4" s="10" t="e">
         <f>GASTOS!F22</f>
-        <v>4485960</v>
-      </c>
-      <c r="G4" s="70"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="72"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G4" s="76"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="78"/>
       <c r="M4" s="2"/>
       <c r="N4" s="3"/>
     </row>
@@ -1765,10 +1813,10 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="10"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="78"/>
     </row>
     <row r="6" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="7" t="s">
@@ -1776,10 +1824,10 @@
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="11"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="72"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="78"/>
     </row>
     <row r="7" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="7" t="s">
@@ -1789,10 +1837,10 @@
       <c r="E7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="70"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="72"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="78"/>
     </row>
     <row r="8" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="7" t="s">
@@ -1800,10 +1848,10 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="12"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="72"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="78"/>
     </row>
     <row r="9" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="7" t="s">
@@ -1811,10 +1859,10 @@
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="12"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="72"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="77"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="78"/>
     </row>
     <row r="10" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="7" t="s">
@@ -1822,10 +1870,10 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="12"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="72"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="78"/>
     </row>
     <row r="11" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="7" t="s">
@@ -1833,10 +1881,10 @@
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="12"/>
-      <c r="G11" s="70"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="72"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="78"/>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1847,10 +1895,10 @@
       <c r="E12" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="70"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="72"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="78"/>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.2">
@@ -1859,10 +1907,10 @@
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="12"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="72"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="78"/>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.2">
@@ -1870,13 +1918,11 @@
         <v>13</v>
       </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="70"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="72"/>
+      <c r="E14" s="54"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="78"/>
       <c r="L14" s="2"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -1887,10 +1933,10 @@
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="12"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="75"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="81"/>
       <c r="L15" s="2"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
@@ -1913,13 +1959,11 @@
       <c r="N16" s="3"/>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="77"/>
-      <c r="E17" s="60" t="s">
-        <v>132</v>
-      </c>
+      <c r="D17" s="83"/>
+      <c r="E17" s="60"/>
       <c r="F17" s="63"/>
       <c r="M17" s="18"/>
       <c r="O17" s="2"/>
@@ -3316,7 +3360,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7A65DF86-7E03-4E93-81F6-CBA0E4BED705}">
           <x14:formula1>
-            <xm:f>TARIFAS!$A$2:$A$54</xm:f>
+            <xm:f>TARIFAS!$A$2:$A$55</xm:f>
           </x14:formula1>
           <xm:sqref>E14</xm:sqref>
         </x14:dataValidation>
@@ -3330,8 +3374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A82BDF-4B1A-4248-B7D7-0A123242CAD7}">
   <dimension ref="C6:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3353,9 +3397,9 @@
       <c r="E6" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="51" t="str">
+      <c r="F6" s="51">
         <f>SOLICITUD!E14</f>
-        <v>BUCARAMANGA</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="3:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3393,12 +3437,12 @@
       <c r="F10" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="78" t="s">
-        <v>134</v>
-      </c>
-      <c r="I10" s="81"/>
-      <c r="J10" s="82"/>
-      <c r="K10" s="83"/>
+      <c r="H10" s="84" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" s="87"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="89"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11" s="33" t="s">
@@ -3407,18 +3451,18 @@
       <c r="D11" s="53">
         <v>1</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="34" t="e">
         <f>VLOOKUP(F6,TARIFAS!A:I,2,FALSE)</f>
-        <v>830180</v>
-      </c>
-      <c r="F11" s="56">
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="56" t="e">
         <f>D11*E11</f>
-        <v>830180</v>
-      </c>
-      <c r="H11" s="79"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="86"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H11" s="85"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="92"/>
     </row>
     <row r="12" spans="3:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="33" t="s">
@@ -3427,18 +3471,18 @@
       <c r="D12" s="53">
         <v>1</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="34" t="e">
         <f>VLOOKUP(F6,TARIFAS!A:I,3,FALSE)</f>
-        <v>70000</v>
-      </c>
-      <c r="F12" s="56">
+        <v>#N/A</v>
+      </c>
+      <c r="F12" s="56" t="e">
         <f t="shared" ref="F12:F13" si="0">D12*E12</f>
-        <v>70000</v>
-      </c>
-      <c r="H12" s="79"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="85"/>
-      <c r="K12" s="86"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H12" s="85"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="92"/>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C13" s="33" t="s">
@@ -3447,18 +3491,18 @@
       <c r="D13" s="53">
         <v>1</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="34" t="e">
         <f>VLOOKUP(F6,TARIFAS!A:I,4,FALSE)</f>
-        <v>90000</v>
-      </c>
-      <c r="F13" s="56">
+        <v>#N/A</v>
+      </c>
+      <c r="F13" s="56" t="e">
         <f t="shared" si="0"/>
-        <v>90000</v>
-      </c>
-      <c r="H13" s="79"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="85"/>
-      <c r="K13" s="86"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H13" s="85"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="92"/>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C14" s="33" t="s">
@@ -3468,18 +3512,18 @@
         <f>D6</f>
         <v>5</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="35" t="e">
         <f>VLOOKUP(F6,TARIFAS!A:I,5,FALSE)</f>
-        <v>60000</v>
-      </c>
-      <c r="F14" s="56">
+        <v>#N/A</v>
+      </c>
+      <c r="F14" s="56" t="e">
         <f>D14*E14</f>
-        <v>300000</v>
-      </c>
-      <c r="H14" s="79"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="85"/>
-      <c r="K14" s="86"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H14" s="85"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="92"/>
     </row>
     <row r="15" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="33" t="s">
@@ -3488,18 +3532,18 @@
       <c r="D15" s="53">
         <v>1</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="34" t="e">
         <f>VLOOKUP(F6,TARIFAS!A:I,6,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="56">
+        <v>#N/A</v>
+      </c>
+      <c r="F15" s="56" t="e">
         <f>D15*E15</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="80"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="89"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H15" s="86"/>
+      <c r="I15" s="93"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="95"/>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C16" s="33" t="s">
@@ -3509,13 +3553,13 @@
         <f>IF(D7&lt;1,0,4*D6/D7)</f>
         <v>10</v>
       </c>
-      <c r="E16" s="36">
+      <c r="E16" s="36" t="e">
         <f>VLOOKUP(F6,TARIFAS!A:I,7,FALSE)</f>
-        <v>20000</v>
-      </c>
-      <c r="F16" s="57">
+        <v>#N/A</v>
+      </c>
+      <c r="F16" s="57" t="e">
         <f>D16*E16</f>
-        <v>200000</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
@@ -3525,13 +3569,13 @@
       <c r="D17" s="53">
         <v>1</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E17" s="36" t="e">
         <f>VLOOKUP(F6,TARIFAS!A:I,8,FALSE)</f>
-        <v>15000</v>
-      </c>
-      <c r="F17" s="56">
+        <v>#N/A</v>
+      </c>
+      <c r="F17" s="56" t="e">
         <f>D17*E17</f>
-        <v>15000</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
@@ -3542,18 +3586,18 @@
         <f>D6-1</f>
         <v>4</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="36" t="e">
         <f>VLOOKUP(F6,TARIFAS!A:I,9,FALSE)</f>
-        <v>184450</v>
-      </c>
-      <c r="F18" s="56">
+        <v>#N/A</v>
+      </c>
+      <c r="F18" s="56" t="e">
         <f>IF(D18&lt;0,0,E18*D18)</f>
-        <v>737800</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D19" s="53">
         <v>0</v>
@@ -3576,18 +3620,18 @@
       <c r="E21" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="37">
+      <c r="F21" s="37" t="e">
         <f>SUM(F11:F18)</f>
-        <v>2242980</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E22" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="37">
+      <c r="F22" s="37" t="e">
         <f>(F21*D7)+F19</f>
-        <v>4485960</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -3604,10 +3648,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278F8443-6907-472D-B3AF-2CF3F50F5416}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3660,7 +3704,6 @@
         <v>0</v>
       </c>
       <c r="C2" s="45">
-        <f t="shared" ref="C2:C34" si="0">35000*2</f>
         <v>70000</v>
       </c>
       <c r="D2" s="46">
@@ -3690,7 +3733,6 @@
         <v>700000</v>
       </c>
       <c r="C3" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D3" s="46">
@@ -3720,7 +3762,6 @@
         <v>0</v>
       </c>
       <c r="C4" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D4" s="46">
@@ -3750,7 +3791,6 @@
         <v>1218100</v>
       </c>
       <c r="C5" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D5" s="46">
@@ -3780,7 +3820,6 @@
         <v>0</v>
       </c>
       <c r="C6" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D6" s="46">
@@ -3806,11 +3845,10 @@
       <c r="A7" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="47">
         <v>772900</v>
       </c>
       <c r="C7" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D7" s="46">
@@ -3837,29 +3875,26 @@
         <v>78</v>
       </c>
       <c r="B8" s="45">
-        <v>0</v>
+        <v>1050000</v>
       </c>
       <c r="C8" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D8" s="46">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="E8" s="45">
-        <v>0</v>
-      </c>
-      <c r="F8" s="45">
-        <v>0</v>
-      </c>
+        <v>60000</v>
+      </c>
+      <c r="F8" s="45"/>
       <c r="G8" s="45">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="H8" s="45">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="I8" s="45">
-        <v>0</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3870,7 +3905,6 @@
         <v>735080</v>
       </c>
       <c r="C9" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D9" s="46">
@@ -3893,18 +3927,16 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="48" t="s">
         <v>80</v>
       </c>
       <c r="B10" s="45">
         <v>0</v>
       </c>
       <c r="C10" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D10" s="46">
-        <f>25000*2</f>
         <v>50000</v>
       </c>
       <c r="E10" s="45">
@@ -3916,7 +3948,7 @@
       <c r="G10" s="45">
         <v>0</v>
       </c>
-      <c r="H10" s="45">
+      <c r="H10" s="46">
         <v>0</v>
       </c>
       <c r="I10" s="45">
@@ -3931,11 +3963,9 @@
         <v>830180</v>
       </c>
       <c r="C11" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D11" s="46">
-        <f>45000*2</f>
         <v>90000</v>
       </c>
       <c r="E11" s="45">
@@ -3962,7 +3992,6 @@
         <v>0</v>
       </c>
       <c r="C12" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D12" s="46">
@@ -3992,11 +4021,9 @@
         <v>584680</v>
       </c>
       <c r="C13" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D13" s="46">
-        <f>75000*2</f>
         <v>150000</v>
       </c>
       <c r="E13" s="45">
@@ -4023,11 +4050,9 @@
         <v>1037930</v>
       </c>
       <c r="C14" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D14" s="46">
-        <f>25000*2</f>
         <v>50000</v>
       </c>
       <c r="E14" s="45">
@@ -4054,7 +4079,6 @@
         <v>0</v>
       </c>
       <c r="C15" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D15" s="46">
@@ -4080,61 +4104,31 @@
       <c r="A16" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="45">
-        <v>0</v>
-      </c>
+      <c r="B16" s="45"/>
       <c r="C16" s="45">
-        <f t="shared" si="0"/>
-        <v>70000</v>
-      </c>
-      <c r="D16" s="46">
-        <v>0</v>
-      </c>
-      <c r="E16" s="45">
-        <v>0</v>
-      </c>
-      <c r="F16" s="45">
-        <v>0</v>
-      </c>
-      <c r="G16" s="45">
-        <v>0</v>
-      </c>
-      <c r="H16" s="45">
-        <v>0</v>
-      </c>
-      <c r="I16" s="45">
-        <v>0</v>
-      </c>
+        <v>70000</v>
+      </c>
+      <c r="D16" s="46"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A17" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="45">
-        <v>0</v>
-      </c>
+      <c r="B17" s="45"/>
       <c r="C17" s="45">
-        <f t="shared" si="0"/>
-        <v>70000</v>
-      </c>
-      <c r="D17" s="46">
-        <v>0</v>
-      </c>
-      <c r="E17" s="45">
-        <v>0</v>
-      </c>
-      <c r="F17" s="45">
-        <v>0</v>
-      </c>
-      <c r="G17" s="45">
-        <v>0</v>
-      </c>
-      <c r="H17" s="45">
-        <v>0</v>
-      </c>
-      <c r="I17" s="45">
-        <v>0</v>
-      </c>
+        <v>70000</v>
+      </c>
+      <c r="D17" s="46"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" s="44" t="s">
@@ -4144,7 +4138,6 @@
         <v>801500</v>
       </c>
       <c r="C18" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D18" s="46">
@@ -4170,11 +4163,10 @@
       <c r="A19" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19" s="45">
         <v>808680</v>
       </c>
       <c r="C19" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D19" s="46">
@@ -4204,7 +4196,6 @@
         <v>0</v>
       </c>
       <c r="C20" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D20" s="46">
@@ -4234,7 +4225,6 @@
         <v>0</v>
       </c>
       <c r="C21" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D21" s="46">
@@ -4264,7 +4254,6 @@
         <v>0</v>
       </c>
       <c r="C22" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D22" s="46">
@@ -4294,7 +4283,6 @@
         <v>1111800</v>
       </c>
       <c r="C23" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D23" s="46">
@@ -4324,7 +4312,6 @@
         <v>0</v>
       </c>
       <c r="C24" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D24" s="46">
@@ -4354,7 +4341,6 @@
         <v>0</v>
       </c>
       <c r="C25" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D25" s="46">
@@ -4384,7 +4370,6 @@
         <v>0</v>
       </c>
       <c r="C26" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D26" s="46">
@@ -4414,7 +4399,6 @@
         <v>0</v>
       </c>
       <c r="C27" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D27" s="46">
@@ -4440,31 +4424,16 @@
       <c r="A28" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="45">
-        <v>0</v>
-      </c>
+      <c r="B28" s="45"/>
       <c r="C28" s="45">
-        <f t="shared" si="0"/>
-        <v>70000</v>
-      </c>
-      <c r="D28" s="46">
-        <v>0</v>
-      </c>
-      <c r="E28" s="45">
-        <v>0</v>
-      </c>
-      <c r="F28" s="45">
-        <v>0</v>
-      </c>
-      <c r="G28" s="45">
-        <v>0</v>
-      </c>
-      <c r="H28" s="45">
-        <v>0</v>
-      </c>
-      <c r="I28" s="45">
-        <v>0</v>
-      </c>
+        <v>70000</v>
+      </c>
+      <c r="D28" s="46"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A29" s="44" t="s">
@@ -4474,7 +4443,6 @@
         <v>718850</v>
       </c>
       <c r="C29" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D29" s="46">
@@ -4504,11 +4472,9 @@
         <v>712980</v>
       </c>
       <c r="C30" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D30" s="46">
-        <f>100000*2</f>
         <v>200000</v>
       </c>
       <c r="E30" s="45">
@@ -4535,11 +4501,9 @@
         <v>774260</v>
       </c>
       <c r="C31" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D31" s="46">
-        <f>30000*2</f>
         <v>60000</v>
       </c>
       <c r="E31" s="45">
@@ -4559,14 +4523,13 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="44" t="s">
         <v>102</v>
       </c>
       <c r="B32" s="45">
         <v>836550</v>
       </c>
       <c r="C32" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D32" s="46">
@@ -4589,14 +4552,13 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="48" t="s">
         <v>103</v>
       </c>
       <c r="B33" s="45">
         <v>0</v>
       </c>
       <c r="C33" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D33" s="46">
@@ -4626,7 +4588,6 @@
         <v>657450</v>
       </c>
       <c r="C34" s="45">
-        <f t="shared" si="0"/>
         <v>70000</v>
       </c>
       <c r="D34" s="46">
@@ -4635,9 +4596,7 @@
       <c r="E34" s="45">
         <v>60000</v>
       </c>
-      <c r="F34" s="45">
-        <v>0</v>
-      </c>
+      <c r="F34" s="45"/>
       <c r="G34" s="45">
         <v>20000</v>
       </c>
@@ -4670,9 +4629,7 @@
       <c r="G35" s="45">
         <v>10000</v>
       </c>
-      <c r="H35" s="45">
-        <v>0</v>
-      </c>
+      <c r="H35" s="45"/>
       <c r="I35" s="45">
         <v>130000</v>
       </c>
@@ -4685,7 +4642,6 @@
         <v>1201220</v>
       </c>
       <c r="C36" s="45">
-        <f t="shared" ref="C36:C54" si="1">35000*2</f>
         <v>70000</v>
       </c>
       <c r="D36" s="46">
@@ -4694,9 +4650,7 @@
       <c r="E36" s="45">
         <v>60000</v>
       </c>
-      <c r="F36" s="45">
-        <v>0</v>
-      </c>
+      <c r="F36" s="45"/>
       <c r="G36" s="45">
         <v>20000</v>
       </c>
@@ -4715,7 +4669,6 @@
         <v>718850</v>
       </c>
       <c r="C37" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D37" s="46">
@@ -4745,7 +4698,6 @@
         <v>0</v>
       </c>
       <c r="C38" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D38" s="46">
@@ -4775,7 +4727,6 @@
         <v>829610</v>
       </c>
       <c r="C39" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D39" s="46">
@@ -4798,134 +4749,129 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="B40" s="45">
-        <v>0</v>
-      </c>
-      <c r="C40" s="45">
-        <f t="shared" si="1"/>
-        <v>70000</v>
-      </c>
-      <c r="D40" s="46">
+      <c r="A40" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="65">
+        <v>712980</v>
+      </c>
+      <c r="C40" s="65">
+        <v>70000</v>
+      </c>
+      <c r="D40" s="65">
         <v>30000</v>
       </c>
-      <c r="E40" s="45">
-        <v>60000</v>
-      </c>
-      <c r="F40" s="45">
-        <v>0</v>
-      </c>
-      <c r="G40" s="45">
+      <c r="E40" s="65">
+        <v>60000</v>
+      </c>
+      <c r="F40" s="65">
+        <v>70000</v>
+      </c>
+      <c r="G40" s="65">
         <v>10000</v>
       </c>
-      <c r="H40" s="45">
-        <v>0</v>
-      </c>
-      <c r="I40" s="45">
-        <v>0</v>
+      <c r="H40" s="65">
+        <v>15000</v>
+      </c>
+      <c r="I40" s="65">
+        <v>130000</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A41" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B41" s="45">
-        <v>795950</v>
+        <v>0</v>
       </c>
       <c r="C41" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D41" s="46">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="E41" s="45">
-        <v>70000</v>
+        <v>60000</v>
       </c>
       <c r="F41" s="45">
         <v>0</v>
       </c>
       <c r="G41" s="45">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="H41" s="45">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="I41" s="45">
-        <v>166897</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A42" s="44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B42" s="45">
-        <v>0</v>
+        <v>795950</v>
       </c>
       <c r="C42" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D42" s="46">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="E42" s="45">
-        <v>60000</v>
+        <v>70000</v>
       </c>
       <c r="F42" s="45">
-        <v>80000</v>
+        <v>0</v>
       </c>
       <c r="G42" s="45">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="H42" s="45">
         <v>15000</v>
       </c>
       <c r="I42" s="45">
-        <v>100000</v>
+        <v>166897</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A43" s="44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" s="45">
-        <v>923800</v>
+        <v>0</v>
       </c>
       <c r="C43" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D43" s="46">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="E43" s="45">
         <v>60000</v>
       </c>
       <c r="F43" s="45">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="G43" s="45">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="H43" s="45">
         <v>15000</v>
       </c>
       <c r="I43" s="45">
-        <v>142480</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A44" s="44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B44" s="45">
-        <v>820940</v>
+        <v>923800</v>
       </c>
       <c r="C44" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D44" s="46">
@@ -4935,217 +4881,194 @@
         <v>60000</v>
       </c>
       <c r="F44" s="45">
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="G44" s="45">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="H44" s="45">
         <v>15000</v>
       </c>
       <c r="I44" s="45">
-        <v>110000</v>
+        <v>142480</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A45" s="44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B45" s="45">
-        <v>0</v>
+        <v>820940</v>
       </c>
       <c r="C45" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D45" s="46">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="E45" s="45">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="F45" s="45">
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="G45" s="45">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="H45" s="45">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="I45" s="45">
-        <v>0</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A46" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="45"/>
+      <c r="C46" s="45">
+        <v>70000</v>
+      </c>
+      <c r="D46" s="46"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="45"/>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="45">
+      <c r="B47" s="45">
         <v>852200</v>
       </c>
-      <c r="C46" s="45">
-        <f t="shared" si="1"/>
-        <v>70000</v>
-      </c>
-      <c r="D46" s="46">
-        <v>60000</v>
-      </c>
-      <c r="E46" s="45">
-        <v>60000</v>
-      </c>
-      <c r="F46" s="45">
+      <c r="C47" s="45">
+        <v>70000</v>
+      </c>
+      <c r="D47" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E47" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F47" s="45">
         <v>100000</v>
       </c>
-      <c r="G46" s="45">
+      <c r="G47" s="45">
         <v>10000</v>
       </c>
-      <c r="H46" s="45">
+      <c r="H47" s="45">
         <v>15000</v>
       </c>
-      <c r="I46" s="45">
+      <c r="I47" s="45">
         <v>110000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="48" t="s">
-        <v>117</v>
-      </c>
-      <c r="B47" s="45">
-        <v>969280</v>
-      </c>
-      <c r="C47" s="45">
-        <f t="shared" si="1"/>
-        <v>70000</v>
-      </c>
-      <c r="D47" s="46">
-        <v>60000</v>
-      </c>
-      <c r="E47" s="45">
-        <v>60000</v>
-      </c>
-      <c r="F47" s="45">
-        <v>0</v>
-      </c>
-      <c r="G47" s="45">
-        <v>20000</v>
-      </c>
-      <c r="H47" s="46">
-        <v>15000</v>
-      </c>
-      <c r="I47" s="45">
-        <v>220000</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A48" s="44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B48" s="45">
-        <v>0</v>
+        <v>969280</v>
       </c>
       <c r="C48" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D48" s="46">
-        <v>30000</v>
+        <v>60000</v>
       </c>
       <c r="E48" s="45">
         <v>60000</v>
       </c>
       <c r="F48" s="45">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="G48" s="45">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="H48" s="45">
         <v>15000</v>
       </c>
       <c r="I48" s="45">
-        <v>85800</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="B49" s="45">
-        <v>0</v>
-      </c>
-      <c r="C49" s="45">
-        <f t="shared" si="1"/>
-        <v>70000</v>
-      </c>
-      <c r="D49" s="46">
-        <v>40000</v>
-      </c>
-      <c r="E49" s="45">
-        <v>60000</v>
-      </c>
-      <c r="F49" s="45">
-        <v>80000</v>
-      </c>
-      <c r="G49" s="45">
+        <v>220000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="70" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" s="67">
+        <v>805000</v>
+      </c>
+      <c r="C49" s="67">
+        <v>70000</v>
+      </c>
+      <c r="D49" s="68">
+        <v>30000</v>
+      </c>
+      <c r="E49" s="69">
+        <v>60000</v>
+      </c>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69">
         <v>20000</v>
       </c>
-      <c r="H49" s="45">
+      <c r="H49" s="69">
         <v>15000</v>
       </c>
-      <c r="I49" s="45">
-        <v>119000</v>
+      <c r="I49" s="69">
+        <v>169900</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B50" s="45">
         <v>0</v>
       </c>
       <c r="C50" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D50" s="46">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="E50" s="45">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="F50" s="45">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="G50" s="45">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="H50" s="45">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="I50" s="45">
-        <v>0</v>
+        <v>85800</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B51" s="45">
-        <v>804120</v>
+        <v>0</v>
       </c>
       <c r="C51" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D51" s="46">
-        <v>60000</v>
+        <v>40000</v>
       </c>
       <c r="E51" s="45">
         <v>60000</v>
       </c>
       <c r="F51" s="45">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="G51" s="45">
         <v>20000</v>
@@ -5154,48 +5077,32 @@
         <v>15000</v>
       </c>
       <c r="I51" s="45">
-        <v>154700</v>
+        <v>119000</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="B52" s="45">
-        <v>0</v>
-      </c>
+      <c r="A52" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" s="45"/>
       <c r="C52" s="45">
-        <f t="shared" si="1"/>
-        <v>70000</v>
-      </c>
-      <c r="D52" s="46">
-        <v>20000</v>
-      </c>
-      <c r="E52" s="45">
-        <v>35000</v>
-      </c>
-      <c r="F52" s="45">
-        <v>40000</v>
-      </c>
-      <c r="G52" s="45">
-        <v>10000</v>
-      </c>
-      <c r="H52" s="45">
-        <v>15000</v>
-      </c>
-      <c r="I52" s="45">
-        <v>0</v>
-      </c>
+        <v>70000</v>
+      </c>
+      <c r="D52" s="46"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="45"/>
     </row>
     <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A53" s="44" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B53" s="45">
-        <v>574350</v>
+        <v>804120</v>
       </c>
       <c r="C53" s="45">
-        <f t="shared" si="1"/>
         <v>70000</v>
       </c>
       <c r="D53" s="46">
@@ -5214,40 +5121,127 @@
         <v>15000</v>
       </c>
       <c r="I53" s="45">
+        <v>154700</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="65">
+        <v>377000</v>
+      </c>
+      <c r="C54" s="65">
+        <v>70000</v>
+      </c>
+      <c r="D54" s="65">
+        <v>50000</v>
+      </c>
+      <c r="E54" s="65">
+        <v>60000</v>
+      </c>
+      <c r="F54" s="65"/>
+      <c r="G54" s="65">
+        <v>10000</v>
+      </c>
+      <c r="H54" s="65">
+        <v>15000</v>
+      </c>
+      <c r="I54" s="65">
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" s="45">
+        <v>0</v>
+      </c>
+      <c r="C55" s="45">
+        <v>70000</v>
+      </c>
+      <c r="D55" s="46">
+        <v>20000</v>
+      </c>
+      <c r="E55" s="45">
+        <v>35000</v>
+      </c>
+      <c r="F55" s="45">
+        <v>40000</v>
+      </c>
+      <c r="G55" s="45">
+        <v>10000</v>
+      </c>
+      <c r="H55" s="45">
+        <v>15000</v>
+      </c>
+      <c r="I55" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56" s="45">
+        <v>574350</v>
+      </c>
+      <c r="C56" s="45">
+        <v>70000</v>
+      </c>
+      <c r="D56" s="46">
+        <v>60000</v>
+      </c>
+      <c r="E56" s="45">
+        <v>60000</v>
+      </c>
+      <c r="F56" s="45">
+        <v>0</v>
+      </c>
+      <c r="G56" s="45">
+        <v>20000</v>
+      </c>
+      <c r="H56" s="45">
+        <v>15000</v>
+      </c>
+      <c r="I56" s="45">
         <v>90000</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="49" t="s">
+    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="B54" s="45">
-        <v>0</v>
-      </c>
-      <c r="C54" s="45">
-        <f t="shared" si="1"/>
-        <v>70000</v>
-      </c>
-      <c r="D54" s="46">
+      <c r="B57" s="45">
+        <v>0</v>
+      </c>
+      <c r="C57" s="45">
+        <v>70000</v>
+      </c>
+      <c r="D57" s="46">
         <v>30000</v>
       </c>
-      <c r="E54" s="45">
+      <c r="E57" s="45">
         <v>35000</v>
       </c>
-      <c r="F54" s="45">
+      <c r="F57" s="45">
         <v>25000</v>
       </c>
-      <c r="G54" s="45">
+      <c r="G57" s="45">
         <v>10000</v>
       </c>
-      <c r="H54" s="45">
+      <c r="H57" s="45">
         <v>15000</v>
       </c>
-      <c r="I54" s="45">
+      <c r="I57" s="45">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I57">
+    <sortCondition ref="A2:A57"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5267,19 +5261,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
     </row>
     <row r="4" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="3:13" x14ac:dyDescent="0.25">
@@ -5303,10 +5297,10 @@
       </c>
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="66"/>
+      <c r="D7" s="72"/>
       <c r="E7" s="10"/>
       <c r="F7" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
v2.0 Style eliminado y CSV agregado
</commit_message>
<xml_diff>
--- a/bdpl/SP.xlsx
+++ b/bdpl/SP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.herrera\programmingProjects\ofertaElectroInterfaz\bdpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1A14E8-BE70-43B1-93DE-9D41B650D611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B9B470-294C-4C6A-BEF0-3153522A1D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1890" windowWidth="29040" windowHeight="15720" xr2:uid="{D648EDC0-5B86-4BF2-94F1-4B01206086EC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{D648EDC0-5B86-4BF2-94F1-4B01206086EC}"/>
   </bookViews>
   <sheets>
     <sheet name="SOLICITUD" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="137">
   <si>
     <t>ESTAMPILLAS</t>
   </si>
@@ -1741,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BFF3BA-D898-4517-B0F1-00F08A29B046}">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1796,9 +1796,9 @@
         <v>3</v>
       </c>
       <c r="D4" s="72"/>
-      <c r="E4" s="10" t="e">
+      <c r="E4" s="10">
         <f>GASTOS!F22</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="G4" s="76"/>
       <c r="H4" s="77"/>
@@ -1918,7 +1918,9 @@
         <v>13</v>
       </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="54"/>
+      <c r="E14" s="54" t="s">
+        <v>80</v>
+      </c>
       <c r="G14" s="76"/>
       <c r="H14" s="77"/>
       <c r="I14" s="77"/>
@@ -3374,8 +3376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A82BDF-4B1A-4248-B7D7-0A123242CAD7}">
   <dimension ref="C6:K22"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3392,14 +3394,14 @@
         <v>53</v>
       </c>
       <c r="D6" s="52">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="51">
+      <c r="F6" s="51" t="str">
         <f>SOLICITUD!E14</f>
-        <v>0</v>
+        <v>BOGOTÁ</v>
       </c>
     </row>
     <row r="7" spans="3:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3407,7 +3409,7 @@
         <v>54</v>
       </c>
       <c r="D7" s="52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="29"/>
@@ -3451,13 +3453,13 @@
       <c r="D11" s="53">
         <v>1</v>
       </c>
-      <c r="E11" s="34" t="e">
+      <c r="E11" s="34">
         <f>VLOOKUP(F6,TARIFAS!A:I,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F11" s="56" t="e">
+        <v>0</v>
+      </c>
+      <c r="F11" s="56">
         <f>D11*E11</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="H11" s="85"/>
       <c r="I11" s="90"/>
@@ -3471,13 +3473,13 @@
       <c r="D12" s="53">
         <v>1</v>
       </c>
-      <c r="E12" s="34" t="e">
+      <c r="E12" s="34">
         <f>VLOOKUP(F6,TARIFAS!A:I,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F12" s="56" t="e">
+        <v>0</v>
+      </c>
+      <c r="F12" s="56">
         <f t="shared" ref="F12:F13" si="0">D12*E12</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="H12" s="85"/>
       <c r="I12" s="90"/>
@@ -3491,13 +3493,13 @@
       <c r="D13" s="53">
         <v>1</v>
       </c>
-      <c r="E13" s="34" t="e">
+      <c r="E13" s="34">
         <f>VLOOKUP(F6,TARIFAS!A:I,4,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F13" s="56" t="e">
+        <v>0</v>
+      </c>
+      <c r="F13" s="56">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="H13" s="85"/>
       <c r="I13" s="90"/>
@@ -3510,15 +3512,15 @@
       </c>
       <c r="D14" s="53">
         <f>D6</f>
-        <v>5</v>
-      </c>
-      <c r="E14" s="35" t="e">
+        <v>0</v>
+      </c>
+      <c r="E14" s="35">
         <f>VLOOKUP(F6,TARIFAS!A:I,5,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F14" s="56" t="e">
+        <v>0</v>
+      </c>
+      <c r="F14" s="56">
         <f>D14*E14</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="H14" s="85"/>
       <c r="I14" s="90"/>
@@ -3532,13 +3534,13 @@
       <c r="D15" s="53">
         <v>1</v>
       </c>
-      <c r="E15" s="34" t="e">
+      <c r="E15" s="34">
         <f>VLOOKUP(F6,TARIFAS!A:I,6,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F15" s="56" t="e">
+        <v>0</v>
+      </c>
+      <c r="F15" s="56">
         <f>D15*E15</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="H15" s="86"/>
       <c r="I15" s="93"/>
@@ -3551,15 +3553,15 @@
       </c>
       <c r="D16" s="55">
         <f>IF(D7&lt;1,0,4*D6/D7)</f>
-        <v>10</v>
-      </c>
-      <c r="E16" s="36" t="e">
+        <v>0</v>
+      </c>
+      <c r="E16" s="36">
         <f>VLOOKUP(F6,TARIFAS!A:I,7,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F16" s="57" t="e">
+        <v>0</v>
+      </c>
+      <c r="F16" s="57">
         <f>D16*E16</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
@@ -3569,13 +3571,13 @@
       <c r="D17" s="53">
         <v>1</v>
       </c>
-      <c r="E17" s="36" t="e">
+      <c r="E17" s="36">
         <f>VLOOKUP(F6,TARIFAS!A:I,8,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F17" s="56" t="e">
+        <v>0</v>
+      </c>
+      <c r="F17" s="56">
         <f>D17*E17</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
@@ -3584,15 +3586,15 @@
       </c>
       <c r="D18" s="53">
         <f>D6-1</f>
-        <v>4</v>
-      </c>
-      <c r="E18" s="36" t="e">
+        <v>-1</v>
+      </c>
+      <c r="E18" s="36">
         <f>VLOOKUP(F6,TARIFAS!A:I,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F18" s="56" t="e">
+        <v>0</v>
+      </c>
+      <c r="F18" s="56">
         <f>IF(D18&lt;0,0,E18*D18)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
@@ -3620,18 +3622,18 @@
       <c r="E21" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="37" t="e">
+      <c r="F21" s="37">
         <f>SUM(F11:F18)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E22" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="37" t="e">
+      <c r="F22" s="37">
         <f>(F21*D7)+F19</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3650,8 +3652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278F8443-6907-472D-B3AF-2CF3F50F5416}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3934,10 +3936,10 @@
         <v>0</v>
       </c>
       <c r="C10" s="45">
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="D10" s="46">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="E10" s="45">
         <v>0</v>

</xml_diff>